<commit_message>
Patched output & played around with prerequisite constraint, but no luck >:(
</commit_message>
<xml_diff>
--- a/Schedule-Data.xlsx
+++ b/Schedule-Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\pipe\CourseConnect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D63E7F-CAC2-41FB-B7BF-C2BDC6823E0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC8E0BD-0EF9-43EC-9589-4F922A22A8AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" activeTab="3" xr2:uid="{503009C4-0C10-4696-AB1F-D7C487AD1E49}"/>
   </bookViews>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="80">
   <si>
     <t>Fall</t>
   </si>
@@ -268,9 +268,6 @@
     <t>Semester 8</t>
   </si>
   <si>
-    <t>Objective</t>
-  </si>
-  <si>
     <t>Min Hrs</t>
   </si>
   <si>
@@ -290,6 +287,36 @@
   </si>
   <si>
     <t>Availability Constraint</t>
+  </si>
+  <si>
+    <t>s in S</t>
+  </si>
+  <si>
+    <t>c in C</t>
+  </si>
+  <si>
+    <t>Suppose:</t>
+  </si>
+  <si>
+    <t>s = 2</t>
+  </si>
+  <si>
+    <t>c = MATH2924</t>
+  </si>
+  <si>
+    <t>p in P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sched </t>
+  </si>
+  <si>
+    <t>prereq</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>sched</t>
   </si>
 </sst>
 </file>
@@ -319,7 +346,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -338,14 +365,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF7030A0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -362,11 +383,85 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -389,9 +484,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -400,6 +492,36 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -28240,1135 +28362,1139 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="16.6640625" style="4" customWidth="1"/>
+    <col min="2" max="16384" width="9.06640625" style="4"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="A2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="3">
         <v>1</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="3">
         <v>1</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="3">
         <v>1</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="3">
         <v>1</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="3">
         <v>1</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="3">
         <v>1</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="3">
         <v>1</v>
       </c>
-      <c r="I2" s="1">
+      <c r="I2" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="1">
+      <c r="A3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3">
         <v>1</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="3">
         <v>1</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="3">
         <v>1</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="3">
         <v>1</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="3">
         <v>1</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="3">
         <v>1</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="3">
         <v>1</v>
       </c>
-      <c r="I3" s="1">
+      <c r="I3" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="1">
+      <c r="A4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3">
         <v>1</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="3">
         <v>1</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="3">
         <v>1</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="3">
         <v>1</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="3">
         <v>1</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="3">
         <v>1</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="3">
         <v>1</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="1">
+      <c r="A5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3">
         <v>1</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="3">
         <v>1</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="3">
         <v>1</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="3">
         <v>1</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="3">
         <v>1</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="3">
         <v>1</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="3">
         <v>1</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I5" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="1">
+      <c r="A6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3">
         <v>1</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="3">
         <v>1</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="3">
         <v>1</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="3">
         <v>1</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="3">
         <v>1</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="3">
         <v>1</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="3">
         <v>1</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1">
+      <c r="A7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="3">
         <v>1</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="3">
         <v>1</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="3">
         <v>1</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="3">
         <v>1</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="3">
         <v>1</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="3">
         <v>1</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="3">
         <v>1</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="1">
+      <c r="A8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="3">
         <v>1</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="3">
         <v>1</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="3">
         <v>1</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="3">
         <v>1</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="3">
         <v>1</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="3">
         <v>1</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="3">
         <v>1</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="1">
+      <c r="A9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="3">
         <v>1</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="3">
         <v>1</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="3">
         <v>1</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="3">
         <v>1</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="3">
         <v>1</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="3">
         <v>1</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="3">
         <v>1</v>
       </c>
-      <c r="I9" s="1">
+      <c r="I9" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="1">
+      <c r="A10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="3">
         <v>1</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="3">
         <v>1</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="3">
         <v>1</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="3">
         <v>1</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="3">
         <v>1</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="3">
         <v>1</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I10" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A11" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B11" s="1">
+      <c r="A11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="3">
         <v>1</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="3">
         <v>1</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="3">
         <v>1</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="3">
         <v>1</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="3">
         <v>1</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="3">
         <v>1</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11" s="3">
         <v>1</v>
       </c>
-      <c r="I11" s="1">
+      <c r="I11" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="1">
+      <c r="A12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="3">
         <v>1</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="3">
         <v>1</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="3">
         <v>1</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="3">
         <v>1</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="3">
         <v>1</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="3">
         <v>1</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12" s="3">
         <v>1</v>
       </c>
-      <c r="I12" s="1">
+      <c r="I12" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="1">
+      <c r="A13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="3">
         <v>1</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="3">
         <v>1</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="3">
         <v>1</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="3">
         <v>1</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="3">
         <v>1</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13" s="3">
         <v>1</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H13" s="3">
         <v>1</v>
       </c>
-      <c r="I13" s="1">
+      <c r="I13" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A14" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14" s="1">
+      <c r="A14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="3">
         <v>1</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="3">
         <v>1</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="3">
         <v>1</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="3">
         <v>1</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14" s="3">
         <v>1</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G14" s="3">
         <v>1</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H14" s="3">
         <v>1</v>
       </c>
-      <c r="I14" s="1">
+      <c r="I14" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A15" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="1">
+      <c r="A15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="3">
         <v>1</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="3">
         <v>1</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="3">
         <v>1</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="3">
         <v>1</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15" s="3">
         <v>1</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G15" s="3">
         <v>1</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H15" s="3">
         <v>1</v>
       </c>
-      <c r="I15" s="1">
+      <c r="I15" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A16" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="1">
-        <v>0</v>
-      </c>
-      <c r="C16" s="1">
+      <c r="A16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0</v>
+      </c>
+      <c r="C16" s="3">
         <v>1</v>
       </c>
-      <c r="D16" s="1">
-        <v>0</v>
-      </c>
-      <c r="E16" s="1">
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3">
         <v>1</v>
       </c>
-      <c r="F16" s="1">
-        <v>0</v>
-      </c>
-      <c r="G16" s="1">
+      <c r="F16" s="3">
+        <v>0</v>
+      </c>
+      <c r="G16" s="3">
         <v>1</v>
       </c>
-      <c r="H16" s="1">
-        <v>0</v>
-      </c>
-      <c r="I16" s="1">
+      <c r="H16" s="3">
+        <v>0</v>
+      </c>
+      <c r="I16" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A17" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="1">
-        <v>0</v>
-      </c>
-      <c r="C17" s="1">
+      <c r="A17" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="3">
+        <v>0</v>
+      </c>
+      <c r="C17" s="3">
         <v>1</v>
       </c>
-      <c r="D17" s="1">
-        <v>0</v>
-      </c>
-      <c r="E17" s="1">
+      <c r="D17" s="3">
+        <v>0</v>
+      </c>
+      <c r="E17" s="3">
         <v>1</v>
       </c>
-      <c r="F17" s="1">
-        <v>0</v>
-      </c>
-      <c r="G17" s="1">
+      <c r="F17" s="3">
+        <v>0</v>
+      </c>
+      <c r="G17" s="3">
         <v>1</v>
       </c>
-      <c r="H17" s="1">
-        <v>0</v>
-      </c>
-      <c r="I17" s="1">
+      <c r="H17" s="3">
+        <v>0</v>
+      </c>
+      <c r="I17" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A18" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B18" s="1">
+      <c r="A18" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="3">
         <v>1</v>
       </c>
-      <c r="C18" s="1">
-        <v>0</v>
-      </c>
-      <c r="D18" s="1">
+      <c r="C18" s="3">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3">
         <v>1</v>
       </c>
-      <c r="E18" s="1">
-        <v>0</v>
-      </c>
-      <c r="F18" s="1">
+      <c r="E18" s="3">
+        <v>0</v>
+      </c>
+      <c r="F18" s="3">
         <v>1</v>
       </c>
-      <c r="G18" s="1">
-        <v>0</v>
-      </c>
-      <c r="H18" s="1">
+      <c r="G18" s="3">
+        <v>0</v>
+      </c>
+      <c r="H18" s="3">
         <v>1</v>
       </c>
-      <c r="I18" s="1">
+      <c r="I18" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A19" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B19" s="1">
-        <v>0</v>
-      </c>
-      <c r="C19" s="1">
+      <c r="A19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="3">
+        <v>0</v>
+      </c>
+      <c r="C19" s="3">
         <v>1</v>
       </c>
-      <c r="D19" s="1">
-        <v>0</v>
-      </c>
-      <c r="E19" s="1">
+      <c r="D19" s="3">
+        <v>0</v>
+      </c>
+      <c r="E19" s="3">
         <v>1</v>
       </c>
-      <c r="F19" s="1">
-        <v>0</v>
-      </c>
-      <c r="G19" s="1">
+      <c r="F19" s="3">
+        <v>0</v>
+      </c>
+      <c r="G19" s="3">
         <v>1</v>
       </c>
-      <c r="H19" s="1">
-        <v>0</v>
-      </c>
-      <c r="I19" s="1">
+      <c r="H19" s="3">
+        <v>0</v>
+      </c>
+      <c r="I19" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A20" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B20" s="1">
+      <c r="A20" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="3">
         <v>1</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="3">
         <v>1</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="3">
         <v>1</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20" s="3">
         <v>1</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F20" s="3">
         <v>1</v>
       </c>
-      <c r="G20" s="1">
+      <c r="G20" s="3">
         <v>1</v>
       </c>
-      <c r="H20" s="1">
+      <c r="H20" s="3">
         <v>1</v>
       </c>
-      <c r="I20" s="1">
+      <c r="I20" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A21" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21" s="1">
+      <c r="A21" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="3">
         <v>1</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="3">
         <v>1</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="3">
         <v>1</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21" s="3">
         <v>1</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F21" s="3">
         <v>1</v>
       </c>
-      <c r="G21" s="1">
+      <c r="G21" s="3">
         <v>1</v>
       </c>
-      <c r="H21" s="1">
+      <c r="H21" s="3">
         <v>1</v>
       </c>
-      <c r="I21" s="1">
+      <c r="I21" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A22" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B22" s="1">
+      <c r="A22" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="3">
         <v>1</v>
       </c>
-      <c r="C22" s="1">
-        <v>0</v>
-      </c>
-      <c r="D22" s="1">
+      <c r="C22" s="3">
+        <v>0</v>
+      </c>
+      <c r="D22" s="3">
         <v>1</v>
       </c>
-      <c r="E22" s="1">
-        <v>0</v>
-      </c>
-      <c r="F22" s="1">
+      <c r="E22" s="3">
+        <v>0</v>
+      </c>
+      <c r="F22" s="3">
         <v>1</v>
       </c>
-      <c r="G22" s="1">
-        <v>0</v>
-      </c>
-      <c r="H22" s="1">
+      <c r="G22" s="3">
+        <v>0</v>
+      </c>
+      <c r="H22" s="3">
         <v>1</v>
       </c>
-      <c r="I22" s="1">
+      <c r="I22" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A23" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B23" s="1">
-        <v>0</v>
-      </c>
-      <c r="C23" s="1">
+      <c r="A23" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="3">
+        <v>0</v>
+      </c>
+      <c r="C23" s="3">
         <v>1</v>
       </c>
-      <c r="D23" s="1">
-        <v>0</v>
-      </c>
-      <c r="E23" s="1">
+      <c r="D23" s="3">
+        <v>0</v>
+      </c>
+      <c r="E23" s="3">
         <v>1</v>
       </c>
-      <c r="F23" s="1">
-        <v>0</v>
-      </c>
-      <c r="G23" s="1">
+      <c r="F23" s="3">
+        <v>0</v>
+      </c>
+      <c r="G23" s="3">
         <v>1</v>
       </c>
-      <c r="H23" s="1">
-        <v>0</v>
-      </c>
-      <c r="I23" s="1">
+      <c r="H23" s="3">
+        <v>0</v>
+      </c>
+      <c r="I23" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A24" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B24" s="1">
-        <v>0</v>
-      </c>
-      <c r="C24" s="1">
+      <c r="A24" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="3">
+        <v>0</v>
+      </c>
+      <c r="C24" s="3">
         <v>1</v>
       </c>
-      <c r="D24" s="1">
-        <v>0</v>
-      </c>
-      <c r="E24" s="1">
+      <c r="D24" s="3">
+        <v>0</v>
+      </c>
+      <c r="E24" s="3">
         <v>1</v>
       </c>
-      <c r="F24" s="1">
-        <v>0</v>
-      </c>
-      <c r="G24" s="1">
+      <c r="F24" s="3">
+        <v>0</v>
+      </c>
+      <c r="G24" s="3">
         <v>1</v>
       </c>
-      <c r="H24" s="1">
-        <v>0</v>
-      </c>
-      <c r="I24" s="1">
+      <c r="H24" s="3">
+        <v>0</v>
+      </c>
+      <c r="I24" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A25" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B25" s="1">
+      <c r="A25" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="3">
         <v>1</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="3">
         <v>1</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25" s="3">
         <v>1</v>
       </c>
-      <c r="E25" s="1">
+      <c r="E25" s="3">
         <v>1</v>
       </c>
-      <c r="F25" s="1">
+      <c r="F25" s="3">
         <v>1</v>
       </c>
-      <c r="G25" s="1">
+      <c r="G25" s="3">
         <v>1</v>
       </c>
-      <c r="H25" s="1">
+      <c r="H25" s="3">
         <v>1</v>
       </c>
-      <c r="I25" s="1">
+      <c r="I25" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A26" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B26" s="1">
+      <c r="A26" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="3">
         <v>1</v>
       </c>
-      <c r="C26" s="1">
-        <v>0</v>
-      </c>
-      <c r="D26" s="1">
+      <c r="C26" s="3">
+        <v>0</v>
+      </c>
+      <c r="D26" s="3">
         <v>1</v>
       </c>
-      <c r="E26" s="1">
-        <v>0</v>
-      </c>
-      <c r="F26" s="1">
+      <c r="E26" s="3">
+        <v>0</v>
+      </c>
+      <c r="F26" s="3">
         <v>1</v>
       </c>
-      <c r="G26" s="1">
-        <v>0</v>
-      </c>
-      <c r="H26" s="1">
+      <c r="G26" s="3">
+        <v>0</v>
+      </c>
+      <c r="H26" s="3">
         <v>1</v>
       </c>
-      <c r="I26" s="1">
+      <c r="I26" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A27" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B27" s="1">
+      <c r="A27" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="3">
         <v>1</v>
       </c>
-      <c r="C27" s="1">
-        <v>0</v>
-      </c>
-      <c r="D27" s="1">
+      <c r="C27" s="3">
+        <v>0</v>
+      </c>
+      <c r="D27" s="3">
         <v>1</v>
       </c>
-      <c r="E27" s="1">
-        <v>0</v>
-      </c>
-      <c r="F27" s="1">
+      <c r="E27" s="3">
+        <v>0</v>
+      </c>
+      <c r="F27" s="3">
         <v>1</v>
       </c>
-      <c r="G27" s="1">
-        <v>0</v>
-      </c>
-      <c r="H27" s="1">
+      <c r="G27" s="3">
+        <v>0</v>
+      </c>
+      <c r="H27" s="3">
         <v>1</v>
       </c>
-      <c r="I27" s="1">
+      <c r="I27" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A28" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B28" s="1">
+      <c r="A28" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="3">
         <v>1</v>
       </c>
-      <c r="C28" s="1">
-        <v>0</v>
-      </c>
-      <c r="D28" s="1">
+      <c r="C28" s="3">
+        <v>0</v>
+      </c>
+      <c r="D28" s="3">
         <v>1</v>
       </c>
-      <c r="E28" s="1">
-        <v>0</v>
-      </c>
-      <c r="F28" s="1">
+      <c r="E28" s="3">
+        <v>0</v>
+      </c>
+      <c r="F28" s="3">
         <v>1</v>
       </c>
-      <c r="G28" s="1">
-        <v>0</v>
-      </c>
-      <c r="H28" s="1">
+      <c r="G28" s="3">
+        <v>0</v>
+      </c>
+      <c r="H28" s="3">
         <v>1</v>
       </c>
-      <c r="I28" s="1">
+      <c r="I28" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A29" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B29" s="1">
+      <c r="A29" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" s="3">
         <v>1</v>
       </c>
-      <c r="C29" s="1">
-        <v>0</v>
-      </c>
-      <c r="D29" s="1">
+      <c r="C29" s="3">
+        <v>0</v>
+      </c>
+      <c r="D29" s="3">
         <v>1</v>
       </c>
-      <c r="E29" s="1">
-        <v>0</v>
-      </c>
-      <c r="F29" s="1">
+      <c r="E29" s="3">
+        <v>0</v>
+      </c>
+      <c r="F29" s="3">
         <v>1</v>
       </c>
-      <c r="G29" s="1">
-        <v>0</v>
-      </c>
-      <c r="H29" s="1">
+      <c r="G29" s="3">
+        <v>0</v>
+      </c>
+      <c r="H29" s="3">
         <v>1</v>
       </c>
-      <c r="I29" s="1">
+      <c r="I29" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A30" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B30" s="1">
-        <v>0</v>
-      </c>
-      <c r="C30" s="1">
+      <c r="A30" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="3">
+        <v>0</v>
+      </c>
+      <c r="C30" s="3">
         <v>1</v>
       </c>
-      <c r="D30" s="1">
-        <v>0</v>
-      </c>
-      <c r="E30" s="1">
+      <c r="D30" s="3">
+        <v>0</v>
+      </c>
+      <c r="E30" s="3">
         <v>1</v>
       </c>
-      <c r="F30" s="1">
-        <v>0</v>
-      </c>
-      <c r="G30" s="1">
+      <c r="F30" s="3">
+        <v>0</v>
+      </c>
+      <c r="G30" s="3">
         <v>1</v>
       </c>
-      <c r="H30" s="1">
-        <v>0</v>
-      </c>
-      <c r="I30" s="1">
+      <c r="H30" s="3">
+        <v>0</v>
+      </c>
+      <c r="I30" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A31" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B31" s="1">
-        <v>0</v>
-      </c>
-      <c r="C31" s="1">
+      <c r="A31" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="3">
+        <v>0</v>
+      </c>
+      <c r="C31" s="3">
         <v>1</v>
       </c>
-      <c r="D31" s="1">
-        <v>0</v>
-      </c>
-      <c r="E31" s="1">
+      <c r="D31" s="3">
+        <v>0</v>
+      </c>
+      <c r="E31" s="3">
         <v>1</v>
       </c>
-      <c r="F31" s="1">
-        <v>0</v>
-      </c>
-      <c r="G31" s="1">
+      <c r="F31" s="3">
+        <v>0</v>
+      </c>
+      <c r="G31" s="3">
         <v>1</v>
       </c>
-      <c r="H31" s="1">
-        <v>0</v>
-      </c>
-      <c r="I31" s="1">
+      <c r="H31" s="3">
+        <v>0</v>
+      </c>
+      <c r="I31" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A32" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B32" s="1">
-        <v>0</v>
-      </c>
-      <c r="C32" s="1">
+      <c r="A32" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32" s="3">
+        <v>0</v>
+      </c>
+      <c r="C32" s="3">
         <v>1</v>
       </c>
-      <c r="D32" s="1">
-        <v>0</v>
-      </c>
-      <c r="E32" s="1">
+      <c r="D32" s="3">
+        <v>0</v>
+      </c>
+      <c r="E32" s="3">
         <v>1</v>
       </c>
-      <c r="F32" s="1">
-        <v>0</v>
-      </c>
-      <c r="G32" s="1">
+      <c r="F32" s="3">
+        <v>0</v>
+      </c>
+      <c r="G32" s="3">
         <v>1</v>
       </c>
-      <c r="H32" s="1">
-        <v>0</v>
-      </c>
-      <c r="I32" s="1">
+      <c r="H32" s="3">
+        <v>0</v>
+      </c>
+      <c r="I32" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A33" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B33" s="1">
-        <v>0</v>
-      </c>
-      <c r="C33" s="1">
+      <c r="A33" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" s="3">
+        <v>0</v>
+      </c>
+      <c r="C33" s="3">
         <v>1</v>
       </c>
-      <c r="D33" s="1">
-        <v>0</v>
-      </c>
-      <c r="E33" s="1">
+      <c r="D33" s="3">
+        <v>0</v>
+      </c>
+      <c r="E33" s="3">
         <v>1</v>
       </c>
-      <c r="F33" s="1">
-        <v>0</v>
-      </c>
-      <c r="G33" s="1">
+      <c r="F33" s="3">
+        <v>0</v>
+      </c>
+      <c r="G33" s="3">
         <v>1</v>
       </c>
-      <c r="H33" s="1">
-        <v>0</v>
-      </c>
-      <c r="I33" s="1">
+      <c r="H33" s="3">
+        <v>0</v>
+      </c>
+      <c r="I33" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A34" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B34" s="1">
+      <c r="A34" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" s="3">
         <v>1</v>
       </c>
-      <c r="C34" s="1">
-        <v>0</v>
-      </c>
-      <c r="D34" s="1">
+      <c r="C34" s="3">
+        <v>0</v>
+      </c>
+      <c r="D34" s="3">
         <v>1</v>
       </c>
-      <c r="E34" s="1">
-        <v>0</v>
-      </c>
-      <c r="F34" s="1">
+      <c r="E34" s="3">
+        <v>0</v>
+      </c>
+      <c r="F34" s="3">
         <v>1</v>
       </c>
-      <c r="G34" s="1">
-        <v>0</v>
-      </c>
-      <c r="H34" s="1">
+      <c r="G34" s="3">
+        <v>0</v>
+      </c>
+      <c r="H34" s="3">
         <v>1</v>
       </c>
-      <c r="I34" s="1">
+      <c r="I34" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A35" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B35" s="1">
+      <c r="A35" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35" s="3">
         <v>1</v>
       </c>
-      <c r="C35" s="1">
-        <v>0</v>
-      </c>
-      <c r="D35" s="1">
+      <c r="C35" s="3">
+        <v>0</v>
+      </c>
+      <c r="D35" s="3">
         <v>1</v>
       </c>
-      <c r="E35" s="1">
-        <v>0</v>
-      </c>
-      <c r="F35" s="1">
+      <c r="E35" s="3">
+        <v>0</v>
+      </c>
+      <c r="F35" s="3">
         <v>1</v>
       </c>
-      <c r="G35" s="1">
-        <v>0</v>
-      </c>
-      <c r="H35" s="1">
+      <c r="G35" s="3">
+        <v>0</v>
+      </c>
+      <c r="H35" s="3">
         <v>1</v>
       </c>
-      <c r="I35" s="1">
+      <c r="I35" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A36" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B36" s="1">
+      <c r="A36" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36" s="3">
         <v>1</v>
       </c>
-      <c r="C36" s="1">
-        <v>0</v>
-      </c>
-      <c r="D36" s="1">
+      <c r="C36" s="3">
+        <v>0</v>
+      </c>
+      <c r="D36" s="3">
         <v>1</v>
       </c>
-      <c r="E36" s="1">
-        <v>0</v>
-      </c>
-      <c r="F36" s="1">
+      <c r="E36" s="3">
+        <v>0</v>
+      </c>
+      <c r="F36" s="3">
         <v>1</v>
       </c>
-      <c r="G36" s="1">
-        <v>0</v>
-      </c>
-      <c r="H36" s="1">
+      <c r="G36" s="3">
+        <v>0</v>
+      </c>
+      <c r="H36" s="3">
         <v>1</v>
       </c>
-      <c r="I36" s="1">
+      <c r="I36" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A37" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B37" s="1">
+      <c r="A37" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37" s="3">
         <v>1</v>
       </c>
-      <c r="C37" s="1">
-        <v>0</v>
-      </c>
-      <c r="D37" s="1">
+      <c r="C37" s="3">
+        <v>0</v>
+      </c>
+      <c r="D37" s="3">
         <v>1</v>
       </c>
-      <c r="E37" s="1">
-        <v>0</v>
-      </c>
-      <c r="F37" s="1">
+      <c r="E37" s="3">
+        <v>0</v>
+      </c>
+      <c r="F37" s="3">
         <v>1</v>
       </c>
-      <c r="G37" s="1">
-        <v>0</v>
-      </c>
-      <c r="H37" s="1">
+      <c r="G37" s="3">
+        <v>0</v>
+      </c>
+      <c r="H37" s="3">
         <v>1</v>
       </c>
-      <c r="I37" s="1">
+      <c r="I37" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A38" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B38" s="1">
+      <c r="A38" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B38" s="3">
         <v>1</v>
       </c>
-      <c r="C38" s="1">
+      <c r="C38" s="3">
         <v>1</v>
       </c>
-      <c r="D38" s="1">
+      <c r="D38" s="3">
         <v>1</v>
       </c>
-      <c r="E38" s="1">
+      <c r="E38" s="3">
         <v>1</v>
       </c>
-      <c r="F38" s="1">
+      <c r="F38" s="3">
         <v>1</v>
       </c>
-      <c r="G38" s="1">
+      <c r="G38" s="3">
         <v>1</v>
       </c>
-      <c r="H38" s="1">
+      <c r="H38" s="3">
         <v>1</v>
       </c>
-      <c r="I38" s="1">
+      <c r="I38" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A39" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B39" s="1">
+      <c r="A39" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B39" s="3">
         <v>1</v>
       </c>
-      <c r="C39" s="1">
+      <c r="C39" s="3">
         <v>1</v>
       </c>
-      <c r="D39" s="1">
+      <c r="D39" s="3">
         <v>1</v>
       </c>
-      <c r="E39" s="1">
+      <c r="E39" s="3">
         <v>1</v>
       </c>
-      <c r="F39" s="1">
+      <c r="F39" s="3">
         <v>1</v>
       </c>
-      <c r="G39" s="1">
+      <c r="G39" s="3">
         <v>1</v>
       </c>
-      <c r="H39" s="1">
+      <c r="H39" s="3">
         <v>1</v>
       </c>
-      <c r="I39" s="1">
+      <c r="I39" s="3">
         <v>1</v>
       </c>
     </row>
@@ -29382,8 +29508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7CDD2E9-B0AB-4B78-AAF0-949DF9D7B865}">
   <dimension ref="A1:AN1004"/>
   <sheetViews>
-    <sheetView zoomScale="78" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView zoomScale="60" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -34126,7 +34252,7 @@
       <c r="AL41" s="3"/>
       <c r="AM41" s="3"/>
     </row>
-    <row r="42" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:39" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -34167,14 +34293,18 @@
       <c r="AL42" s="3"/>
       <c r="AM42" s="3"/>
     </row>
-    <row r="43" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:39" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
+      <c r="C43" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D43" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="20"/>
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
       <c r="J43" s="3"/>
@@ -34211,7 +34341,7 @@
     <row r="44" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
+      <c r="C44" s="16"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
@@ -34249,49 +34379,61 @@
       <c r="AL44" s="3"/>
       <c r="AM44" s="3"/>
     </row>
+    <row r="45" spans="1:39" x14ac:dyDescent="0.45">
+      <c r="C45" s="16"/>
+    </row>
+    <row r="46" spans="1:39" x14ac:dyDescent="0.45">
+      <c r="C46" s="16"/>
+    </row>
+    <row r="47" spans="1:39" x14ac:dyDescent="0.45">
+      <c r="C47" s="16"/>
+    </row>
+    <row r="48" spans="1:39" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C48" s="17"/>
+    </row>
     <row r="50" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="B50" s="10"/>
-      <c r="C50" s="10"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="10"/>
-      <c r="F50" s="10"/>
-      <c r="G50" s="10"/>
-      <c r="H50" s="10"/>
-      <c r="I50" s="10"/>
-      <c r="J50" s="10"/>
-      <c r="K50" s="10"/>
-      <c r="L50" s="10"/>
-      <c r="M50" s="10"/>
-      <c r="N50" s="10"/>
-      <c r="O50" s="10"/>
-      <c r="P50" s="10"/>
-      <c r="Q50" s="10"/>
-      <c r="R50" s="10"/>
-      <c r="S50" s="10"/>
-      <c r="T50" s="10"/>
-      <c r="U50" s="10"/>
-      <c r="V50" s="10"/>
-      <c r="W50" s="10"/>
-      <c r="X50" s="10"/>
-      <c r="Y50" s="10"/>
-      <c r="Z50" s="10"/>
-      <c r="AA50" s="10"/>
-      <c r="AB50" s="10"/>
-      <c r="AC50" s="10"/>
-      <c r="AD50" s="10"/>
-      <c r="AE50" s="10"/>
-      <c r="AF50" s="10"/>
-      <c r="AG50" s="10"/>
-      <c r="AH50" s="10"/>
-      <c r="AI50" s="10"/>
-      <c r="AJ50" s="10"/>
-      <c r="AK50" s="10"/>
-      <c r="AL50" s="10"/>
-      <c r="AM50" s="10"/>
-      <c r="AN50" s="10"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9"/>
+      <c r="H50" s="9"/>
+      <c r="I50" s="9"/>
+      <c r="J50" s="9"/>
+      <c r="K50" s="9"/>
+      <c r="L50" s="9"/>
+      <c r="M50" s="9"/>
+      <c r="N50" s="9"/>
+      <c r="O50" s="9"/>
+      <c r="P50" s="9"/>
+      <c r="Q50" s="9"/>
+      <c r="R50" s="9"/>
+      <c r="S50" s="9"/>
+      <c r="T50" s="9"/>
+      <c r="U50" s="9"/>
+      <c r="V50" s="9"/>
+      <c r="W50" s="9"/>
+      <c r="X50" s="9"/>
+      <c r="Y50" s="9"/>
+      <c r="Z50" s="9"/>
+      <c r="AA50" s="9"/>
+      <c r="AB50" s="9"/>
+      <c r="AC50" s="9"/>
+      <c r="AD50" s="9"/>
+      <c r="AE50" s="9"/>
+      <c r="AF50" s="9"/>
+      <c r="AG50" s="9"/>
+      <c r="AH50" s="9"/>
+      <c r="AI50" s="9"/>
+      <c r="AJ50" s="9"/>
+      <c r="AK50" s="9"/>
+      <c r="AL50" s="9"/>
+      <c r="AM50" s="9"/>
+      <c r="AN50" s="9"/>
     </row>
     <row r="51" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A51" s="9"/>
+      <c r="A51" s="8"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
@@ -34333,7 +34475,7 @@
       <c r="AN51" s="3"/>
     </row>
     <row r="52" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A52" s="9"/>
+      <c r="A52" s="8"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
@@ -34375,7 +34517,7 @@
       <c r="AN52" s="3"/>
     </row>
     <row r="53" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A53" s="9"/>
+      <c r="A53" s="8"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
@@ -34417,7 +34559,7 @@
       <c r="AN53" s="3"/>
     </row>
     <row r="54" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A54" s="9"/>
+      <c r="A54" s="8"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
@@ -34459,7 +34601,7 @@
       <c r="AN54" s="3"/>
     </row>
     <row r="55" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A55" s="9"/>
+      <c r="A55" s="8"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
@@ -34501,7 +34643,7 @@
       <c r="AN55" s="3"/>
     </row>
     <row r="56" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A56" s="9"/>
+      <c r="A56" s="8"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
@@ -34543,7 +34685,7 @@
       <c r="AN56" s="3"/>
     </row>
     <row r="57" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A57" s="9"/>
+      <c r="A57" s="8"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
@@ -34585,7 +34727,7 @@
       <c r="AN57" s="3"/>
     </row>
     <row r="58" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A58" s="9"/>
+      <c r="A58" s="8"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
@@ -34627,7 +34769,7 @@
       <c r="AN58" s="3"/>
     </row>
     <row r="59" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A59" s="9"/>
+      <c r="A59" s="8"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
@@ -34669,7 +34811,7 @@
       <c r="AN59" s="3"/>
     </row>
     <row r="60" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A60" s="9"/>
+      <c r="A60" s="8"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
@@ -34711,7 +34853,7 @@
       <c r="AN60" s="3"/>
     </row>
     <row r="61" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A61" s="9"/>
+      <c r="A61" s="8"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
@@ -34752,7 +34894,7 @@
       <c r="AN61" s="3"/>
     </row>
     <row r="62" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A62" s="9"/>
+      <c r="A62" s="8"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
@@ -34794,7 +34936,7 @@
       <c r="AN62" s="3"/>
     </row>
     <row r="63" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A63" s="9"/>
+      <c r="A63" s="8"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
@@ -34836,7 +34978,7 @@
       <c r="AN63" s="3"/>
     </row>
     <row r="64" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A64" s="9"/>
+      <c r="A64" s="8"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
@@ -34878,7 +35020,7 @@
       <c r="AN64" s="3"/>
     </row>
     <row r="65" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A65" s="9"/>
+      <c r="A65" s="8"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
@@ -34920,7 +35062,7 @@
       <c r="AN65" s="3"/>
     </row>
     <row r="66" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A66" s="9"/>
+      <c r="A66" s="8"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
@@ -34962,7 +35104,7 @@
       <c r="AN66" s="3"/>
     </row>
     <row r="67" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A67" s="9"/>
+      <c r="A67" s="8"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
@@ -35004,7 +35146,7 @@
       <c r="AN67" s="3"/>
     </row>
     <row r="68" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A68" s="9"/>
+      <c r="A68" s="8"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
@@ -35046,7 +35188,7 @@
       <c r="AN68" s="3"/>
     </row>
     <row r="69" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A69" s="9"/>
+      <c r="A69" s="8"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
@@ -35088,7 +35230,7 @@
       <c r="AN69" s="3"/>
     </row>
     <row r="70" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A70" s="9"/>
+      <c r="A70" s="8"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
@@ -35130,7 +35272,7 @@
       <c r="AN70" s="3"/>
     </row>
     <row r="71" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A71" s="9"/>
+      <c r="A71" s="8"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
       <c r="D71" s="3"/>
@@ -35172,7 +35314,7 @@
       <c r="AN71" s="3"/>
     </row>
     <row r="72" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A72" s="9"/>
+      <c r="A72" s="8"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
       <c r="D72" s="3"/>
@@ -35214,7 +35356,7 @@
       <c r="AN72" s="3"/>
     </row>
     <row r="73" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A73" s="9"/>
+      <c r="A73" s="8"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
@@ -35256,7 +35398,7 @@
       <c r="AN73" s="3"/>
     </row>
     <row r="74" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A74" s="9"/>
+      <c r="A74" s="8"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
       <c r="D74" s="3"/>
@@ -35298,7 +35440,7 @@
       <c r="AN74" s="3"/>
     </row>
     <row r="75" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A75" s="9"/>
+      <c r="A75" s="8"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
       <c r="D75" s="3"/>
@@ -35340,7 +35482,7 @@
       <c r="AN75" s="3"/>
     </row>
     <row r="76" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A76" s="9"/>
+      <c r="A76" s="8"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
       <c r="D76" s="3"/>
@@ -35382,7 +35524,7 @@
       <c r="AN76" s="3"/>
     </row>
     <row r="77" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A77" s="9"/>
+      <c r="A77" s="8"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
       <c r="D77" s="3"/>
@@ -35424,7 +35566,7 @@
       <c r="AN77" s="3"/>
     </row>
     <row r="78" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A78" s="9"/>
+      <c r="A78" s="8"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
       <c r="D78" s="3"/>
@@ -35466,7 +35608,7 @@
       <c r="AN78" s="3"/>
     </row>
     <row r="79" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A79" s="9"/>
+      <c r="A79" s="8"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
       <c r="D79" s="3"/>
@@ -35508,7 +35650,7 @@
       <c r="AN79" s="3"/>
     </row>
     <row r="80" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A80" s="9"/>
+      <c r="A80" s="8"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
       <c r="D80" s="3"/>
@@ -35550,7 +35692,7 @@
       <c r="AN80" s="3"/>
     </row>
     <row r="81" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A81" s="9"/>
+      <c r="A81" s="8"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
       <c r="D81" s="3"/>
@@ -35592,7 +35734,7 @@
       <c r="AN81" s="3"/>
     </row>
     <row r="82" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A82" s="9"/>
+      <c r="A82" s="8"/>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
       <c r="D82" s="3"/>
@@ -35634,7 +35776,7 @@
       <c r="AN82" s="3"/>
     </row>
     <row r="83" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A83" s="9"/>
+      <c r="A83" s="8"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
       <c r="D83" s="3"/>
@@ -35676,7 +35818,7 @@
       <c r="AN83" s="3"/>
     </row>
     <row r="84" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A84" s="9"/>
+      <c r="A84" s="8"/>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
       <c r="D84" s="3"/>
@@ -35718,7 +35860,7 @@
       <c r="AN84" s="3"/>
     </row>
     <row r="85" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A85" s="9"/>
+      <c r="A85" s="8"/>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
       <c r="D85" s="3"/>
@@ -35760,7 +35902,7 @@
       <c r="AN85" s="3"/>
     </row>
     <row r="86" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A86" s="9"/>
+      <c r="A86" s="8"/>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
       <c r="D86" s="3"/>
@@ -35802,7 +35944,7 @@
       <c r="AN86" s="3"/>
     </row>
     <row r="87" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A87" s="9"/>
+      <c r="A87" s="8"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
       <c r="D87" s="3"/>
@@ -35844,7 +35986,7 @@
       <c r="AN87" s="3"/>
     </row>
     <row r="88" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A88" s="9"/>
+      <c r="A88" s="8"/>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
       <c r="D88" s="3"/>
@@ -35886,7 +36028,7 @@
       <c r="AN88" s="3"/>
     </row>
     <row r="89" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A89" s="9"/>
+      <c r="A89" s="8"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
       <c r="D89" s="3"/>
@@ -73443,24 +73585,31 @@
       <c r="AM1004" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C43:C48"/>
+    <mergeCell ref="D43:G43"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D099514-66A9-40BB-8236-071D2A75DD12}">
-  <dimension ref="A1:O93"/>
+  <dimension ref="A1:Q93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="62" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="16384" width="9.06640625" style="4"/>
+    <col min="1" max="1" width="9.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="14" width="9.06640625" style="4"/>
+    <col min="15" max="15" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.06640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:17" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -73489,32 +73638,35 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="B2" s="5">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5">
+        <v>0</v>
+      </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
-      <c r="N2" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="O2" s="8">
-        <f>MAX(B46:I46)-MIN(B46:I46)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
+        <v>11</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0</v>
+      </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -73522,25 +73674,42 @@
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
+        <v>12</v>
+      </c>
+      <c r="B4" s="5">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0</v>
+      </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="M4" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="B5" s="5">
+        <v>0</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0</v>
+      </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -73548,103 +73717,156 @@
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
+        <v>14</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0</v>
+      </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="M6" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="14"/>
+    </row>
+    <row r="7" spans="1:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
+        <v>15</v>
+      </c>
+      <c r="B7" s="5">
+        <v>0</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0</v>
+      </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="M7" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="N7" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="14"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
+        <v>16</v>
+      </c>
+      <c r="B8" s="5">
+        <v>0</v>
+      </c>
+      <c r="C8" s="5">
+        <v>1</v>
+      </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="M8" s="16"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="B9" s="5">
+        <v>0</v>
+      </c>
+      <c r="C9" s="5">
+        <v>1</v>
+      </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="M9" s="16"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
+        <v>18</v>
+      </c>
+      <c r="B10" s="5">
+        <v>0</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0</v>
+      </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="M10" s="16"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
+        <v>19</v>
+      </c>
+      <c r="B11" s="5">
+        <v>0</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0</v>
+      </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="M11" s="16"/>
+    </row>
+    <row r="12" spans="1:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="B12" s="5">
+        <v>0</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0</v>
+      </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="M12" s="17"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
+        <v>21</v>
+      </c>
+      <c r="B13" s="5">
+        <v>1</v>
+      </c>
+      <c r="C13" s="5">
+        <v>0</v>
+      </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
@@ -73652,12 +73874,16 @@
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
+        <v>22</v>
+      </c>
+      <c r="B14" s="5">
+        <v>0</v>
+      </c>
+      <c r="C14" s="5">
+        <v>1</v>
+      </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
@@ -73665,12 +73891,16 @@
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
+        <v>23</v>
+      </c>
+      <c r="B15" s="5">
+        <v>0</v>
+      </c>
+      <c r="C15" s="5">
+        <v>0</v>
+      </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
@@ -73678,12 +73908,16 @@
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
+        <v>24</v>
+      </c>
+      <c r="B16" s="5">
+        <v>0</v>
+      </c>
+      <c r="C16" s="5">
+        <v>0</v>
+      </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
@@ -73691,12 +73925,16 @@
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="B17" s="5">
+        <v>0</v>
+      </c>
+      <c r="C17" s="5">
+        <v>0</v>
+      </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
@@ -73704,12 +73942,16 @@
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="B18" s="5">
+        <v>1</v>
+      </c>
+      <c r="C18" s="5">
+        <v>0</v>
+      </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
@@ -73717,12 +73959,16 @@
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
+        <v>27</v>
+      </c>
+      <c r="B19" s="5">
+        <v>0</v>
+      </c>
+      <c r="C19" s="5">
+        <v>0</v>
+      </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
@@ -73730,12 +73976,16 @@
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="B20" s="5">
+        <v>0</v>
+      </c>
+      <c r="C20" s="5">
+        <v>0</v>
+      </c>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
@@ -73743,12 +73993,16 @@
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
+        <v>29</v>
+      </c>
+      <c r="B21" s="5">
+        <v>1</v>
+      </c>
+      <c r="C21" s="5">
+        <v>0</v>
+      </c>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
@@ -73756,25 +74010,48 @@
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="B22" s="5">
+        <v>0</v>
+      </c>
+      <c r="C22" s="5">
+        <v>0</v>
+      </c>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="M22" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="N22" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="O22" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="P22" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q22" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="B23" s="5">
+        <v>0</v>
+      </c>
+      <c r="C23" s="5">
+        <v>1</v>
+      </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
@@ -73782,12 +74059,16 @@
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
+        <v>32</v>
+      </c>
+      <c r="B24" s="5">
+        <v>0</v>
+      </c>
+      <c r="C24" s="5">
+        <v>1</v>
+      </c>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
@@ -73795,12 +74076,16 @@
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
+        <v>33</v>
+      </c>
+      <c r="B25" s="5">
+        <v>1</v>
+      </c>
+      <c r="C25" s="5">
+        <v>0</v>
+      </c>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
@@ -73808,12 +74093,16 @@
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A26" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
+        <v>34</v>
+      </c>
+      <c r="B26" s="5">
+        <v>0</v>
+      </c>
+      <c r="C26" s="5">
+        <v>0</v>
+      </c>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
@@ -73821,12 +74110,16 @@
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A27" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
+        <v>35</v>
+      </c>
+      <c r="B27" s="5">
+        <v>0</v>
+      </c>
+      <c r="C27" s="5">
+        <v>0</v>
+      </c>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
@@ -73834,12 +74127,16 @@
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A28" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
+        <v>36</v>
+      </c>
+      <c r="B28" s="5">
+        <v>0</v>
+      </c>
+      <c r="C28" s="5">
+        <v>0</v>
+      </c>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
@@ -73847,12 +74144,16 @@
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A29" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
+        <v>37</v>
+      </c>
+      <c r="B29" s="5">
+        <v>0</v>
+      </c>
+      <c r="C29" s="5">
+        <v>0</v>
+      </c>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
@@ -73860,12 +74161,16 @@
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A30" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
+        <v>38</v>
+      </c>
+      <c r="B30" s="5">
+        <v>0</v>
+      </c>
+      <c r="C30" s="5">
+        <v>0</v>
+      </c>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
@@ -73873,12 +74178,16 @@
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A31" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="B31" s="5">
+        <v>0</v>
+      </c>
+      <c r="C31" s="5">
+        <v>0</v>
+      </c>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
@@ -73886,12 +74195,16 @@
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A32" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
+        <v>40</v>
+      </c>
+      <c r="B32" s="5">
+        <v>0</v>
+      </c>
+      <c r="C32" s="5">
+        <v>0</v>
+      </c>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
@@ -73901,10 +74214,14 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
+        <v>41</v>
+      </c>
+      <c r="B33" s="5">
+        <v>0</v>
+      </c>
+      <c r="C33" s="5">
+        <v>0</v>
+      </c>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
@@ -73914,10 +74231,14 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A34" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
+        <v>42</v>
+      </c>
+      <c r="B34" s="5">
+        <v>0</v>
+      </c>
+      <c r="C34" s="5">
+        <v>0</v>
+      </c>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
@@ -73927,10 +74248,14 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
+        <v>43</v>
+      </c>
+      <c r="B35" s="5">
+        <v>0</v>
+      </c>
+      <c r="C35" s="5">
+        <v>0</v>
+      </c>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
@@ -73940,10 +74265,14 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="B36" s="5">
+        <v>1</v>
+      </c>
+      <c r="C36" s="5">
+        <v>0</v>
+      </c>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
@@ -73953,10 +74282,14 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
+        <v>45</v>
+      </c>
+      <c r="B37" s="5">
+        <v>0</v>
+      </c>
+      <c r="C37" s="5">
+        <v>0</v>
+      </c>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
@@ -73966,10 +74299,14 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A38" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
+        <v>46</v>
+      </c>
+      <c r="B38" s="5">
+        <v>0</v>
+      </c>
+      <c r="C38" s="5">
+        <v>0</v>
+      </c>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
@@ -73979,10 +74316,14 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A39" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="B39" s="5">
+        <v>0</v>
+      </c>
+      <c r="C39" s="5">
+        <v>0</v>
+      </c>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
@@ -73991,21 +74332,21 @@
       <c r="I39" s="5"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A43" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
-      <c r="E43" s="11"/>
-      <c r="F43" s="11"/>
-      <c r="G43" s="11"/>
-      <c r="H43" s="11"/>
-      <c r="I43" s="11"/>
+      <c r="A43" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="10"/>
+      <c r="I43" s="10"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A44" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B44" s="6">
         <v>12</v>
@@ -74034,28 +74375,28 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B45" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.45">
@@ -74064,11 +74405,11 @@
       </c>
       <c r="B46" s="4">
         <f t="shared" ref="B46:I46" si="0">SUM(B2:B39)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C46" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D46" s="4">
         <f t="shared" si="0"/>
@@ -74097,33 +74438,33 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B47" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A48" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B48" s="6">
         <v>20</v>
@@ -74151,19 +74492,19 @@
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A54" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="B54" s="11"/>
-      <c r="C54" s="11"/>
-      <c r="D54" s="11"/>
-      <c r="E54" s="11"/>
-      <c r="F54" s="11"/>
-      <c r="G54" s="11"/>
-      <c r="H54" s="11"/>
-      <c r="I54" s="11"/>
-      <c r="J54" s="11"/>
-      <c r="K54" s="11"/>
+      <c r="A54" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B54" s="10"/>
+      <c r="C54" s="10"/>
+      <c r="D54" s="10"/>
+      <c r="E54" s="10"/>
+      <c r="F54" s="10"/>
+      <c r="G54" s="10"/>
+      <c r="H54" s="10"/>
+      <c r="I54" s="10"/>
+      <c r="J54" s="10"/>
+      <c r="K54" s="10"/>
     </row>
     <row r="55" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A55" s="3" t="s">
@@ -74231,7 +74572,7 @@
         <v>0</v>
       </c>
       <c r="J56" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K56" s="6">
         <v>1</v>
@@ -74274,7 +74615,7 @@
         <v>0</v>
       </c>
       <c r="J57" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K57" s="6">
         <v>1</v>
@@ -74286,7 +74627,7 @@
       </c>
       <c r="B58" s="3">
         <f>B4*'ISE Availability'!B4</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C58" s="3">
         <f>C4*'ISE Availability'!C4</f>
@@ -74317,7 +74658,7 @@
         <v>0</v>
       </c>
       <c r="J58" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K58" s="6">
         <v>1</v>
@@ -74360,7 +74701,7 @@
         <v>0</v>
       </c>
       <c r="J59" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K59" s="6">
         <v>1</v>
@@ -74403,7 +74744,7 @@
         <v>0</v>
       </c>
       <c r="J60" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K60" s="6">
         <v>1</v>
@@ -74446,7 +74787,7 @@
         <v>0</v>
       </c>
       <c r="J61" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K61" s="6">
         <v>1</v>
@@ -74462,7 +74803,7 @@
       </c>
       <c r="C62" s="3">
         <f>C8*'ISE Availability'!C8</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D62" s="3">
         <f>D8*'ISE Availability'!D8</f>
@@ -74489,7 +74830,7 @@
         <v>0</v>
       </c>
       <c r="J62" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K62" s="6">
         <v>1</v>
@@ -74505,7 +74846,7 @@
       </c>
       <c r="C63" s="3">
         <f>C9*'ISE Availability'!C9</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D63" s="3">
         <f>D9*'ISE Availability'!D9</f>
@@ -74532,7 +74873,7 @@
         <v>0</v>
       </c>
       <c r="J63" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K63" s="6">
         <v>1</v>
@@ -74575,7 +74916,7 @@
         <v>0</v>
       </c>
       <c r="J64" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K64" s="6">
         <v>1</v>
@@ -74618,7 +74959,7 @@
         <v>0</v>
       </c>
       <c r="J65" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K65" s="6">
         <v>1</v>
@@ -74661,7 +75002,7 @@
         <v>0</v>
       </c>
       <c r="J66" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K66" s="6">
         <v>1</v>
@@ -74673,7 +75014,7 @@
       </c>
       <c r="B67" s="3">
         <f>B13*'ISE Availability'!B13</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C67" s="3">
         <f>C13*'ISE Availability'!C13</f>
@@ -74704,7 +75045,7 @@
         <v>0</v>
       </c>
       <c r="J67" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K67" s="6">
         <v>1</v>
@@ -74720,7 +75061,7 @@
       </c>
       <c r="C68" s="3">
         <f>C14*'ISE Availability'!C14</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D68" s="3">
         <f>D14*'ISE Availability'!D14</f>
@@ -74747,7 +75088,7 @@
         <v>0</v>
       </c>
       <c r="J68" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K68" s="6">
         <v>1</v>
@@ -74790,7 +75131,7 @@
         <v>0</v>
       </c>
       <c r="J69" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K69" s="6">
         <v>1</v>
@@ -74833,7 +75174,7 @@
         <v>0</v>
       </c>
       <c r="J70" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K70" s="6">
         <v>1</v>
@@ -74876,7 +75217,7 @@
         <v>0</v>
       </c>
       <c r="J71" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K71" s="6">
         <v>1</v>
@@ -74888,7 +75229,7 @@
       </c>
       <c r="B72" s="3">
         <f>B18*'ISE Availability'!B18</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C72" s="3">
         <f>C18*'ISE Availability'!C18</f>
@@ -74919,7 +75260,7 @@
         <v>0</v>
       </c>
       <c r="J72" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K72" s="6">
         <v>1</v>
@@ -74962,7 +75303,7 @@
         <v>0</v>
       </c>
       <c r="J73" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K73" s="6">
         <v>1</v>
@@ -75005,7 +75346,7 @@
         <v>0</v>
       </c>
       <c r="J74" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K74" s="6">
         <v>1</v>
@@ -75017,7 +75358,7 @@
       </c>
       <c r="B75" s="3">
         <f>B21*'ISE Availability'!B21</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C75" s="3">
         <f>C21*'ISE Availability'!C21</f>
@@ -75048,7 +75389,7 @@
         <v>0</v>
       </c>
       <c r="J75" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K75" s="6">
         <v>1</v>
@@ -75091,7 +75432,7 @@
         <v>0</v>
       </c>
       <c r="J76" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K76" s="6">
         <v>1</v>
@@ -75107,7 +75448,7 @@
       </c>
       <c r="C77" s="3">
         <f>C23*'ISE Availability'!C23</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D77" s="3">
         <f>D23*'ISE Availability'!D23</f>
@@ -75134,7 +75475,7 @@
         <v>0</v>
       </c>
       <c r="J77" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K77" s="6">
         <v>1</v>
@@ -75150,7 +75491,7 @@
       </c>
       <c r="C78" s="3">
         <f>C24*'ISE Availability'!C24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D78" s="3">
         <f>D24*'ISE Availability'!D24</f>
@@ -75177,7 +75518,7 @@
         <v>0</v>
       </c>
       <c r="J78" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K78" s="6">
         <v>1</v>
@@ -75189,7 +75530,7 @@
       </c>
       <c r="B79" s="3">
         <f>B25*'ISE Availability'!B25</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C79" s="3">
         <f>C25*'ISE Availability'!C25</f>
@@ -75220,7 +75561,7 @@
         <v>0</v>
       </c>
       <c r="J79" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K79" s="6">
         <v>1</v>
@@ -75263,7 +75604,7 @@
         <v>0</v>
       </c>
       <c r="J80" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K80" s="6">
         <v>1</v>
@@ -75306,7 +75647,7 @@
         <v>0</v>
       </c>
       <c r="J81" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K81" s="6">
         <v>1</v>
@@ -75349,7 +75690,7 @@
         <v>0</v>
       </c>
       <c r="J82" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K82" s="6">
         <v>1</v>
@@ -75392,7 +75733,7 @@
         <v>0</v>
       </c>
       <c r="J83" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K83" s="6">
         <v>1</v>
@@ -75435,7 +75776,7 @@
         <v>0</v>
       </c>
       <c r="J84" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K84" s="6">
         <v>1</v>
@@ -75478,7 +75819,7 @@
         <v>0</v>
       </c>
       <c r="J85" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K85" s="6">
         <v>1</v>
@@ -75521,7 +75862,7 @@
         <v>0</v>
       </c>
       <c r="J86" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K86" s="6">
         <v>1</v>
@@ -75564,7 +75905,7 @@
         <v>0</v>
       </c>
       <c r="J87" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K87" s="6">
         <v>1</v>
@@ -75607,7 +75948,7 @@
         <v>0</v>
       </c>
       <c r="J88" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K88" s="6">
         <v>1</v>
@@ -75650,7 +75991,7 @@
         <v>0</v>
       </c>
       <c r="J89" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K89" s="6">
         <v>1</v>
@@ -75662,7 +76003,7 @@
       </c>
       <c r="B90" s="3">
         <f>B36*'ISE Availability'!B36</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C90" s="3">
         <f>C36*'ISE Availability'!C36</f>
@@ -75693,7 +76034,7 @@
         <v>0</v>
       </c>
       <c r="J90" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K90" s="6">
         <v>1</v>
@@ -75736,7 +76077,7 @@
         <v>0</v>
       </c>
       <c r="J91" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K91" s="6">
         <v>1</v>
@@ -75779,7 +76120,7 @@
         <v>0</v>
       </c>
       <c r="J92" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K92" s="6">
         <v>1</v>
@@ -75822,16 +76163,19 @@
         <v>0</v>
       </c>
       <c r="J93" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K93" s="6">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
     <mergeCell ref="A43:I43"/>
     <mergeCell ref="A54:K54"/>
+    <mergeCell ref="M6:Q6"/>
+    <mergeCell ref="M7:M12"/>
+    <mergeCell ref="N7:Q7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Freshen up before Gonzalez
</commit_message>
<xml_diff>
--- a/Schedule-Data.xlsx
+++ b/Schedule-Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\pipe\CourseConnect\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\pipe\Shaman\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC8E0BD-0EF9-43EC-9589-4F922A22A8AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{142DBEF8-3542-4D69-9C16-01A115B3F931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" activeTab="3" xr2:uid="{503009C4-0C10-4696-AB1F-D7C487AD1E49}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" activeTab="2" xr2:uid="{503009C4-0C10-4696-AB1F-D7C487AD1E49}"/>
   </bookViews>
   <sheets>
     <sheet name="ISE" sheetId="1" r:id="rId1"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="65">
   <si>
     <t>Fall</t>
   </si>
@@ -268,55 +268,10 @@
     <t>Semester 8</t>
   </si>
   <si>
-    <t>Min Hrs</t>
-  </si>
-  <si>
-    <t>Max Hrs</t>
-  </si>
-  <si>
-    <t>&gt;=</t>
-  </si>
-  <si>
-    <t>&lt;=</t>
-  </si>
-  <si>
-    <t>==</t>
-  </si>
-  <si>
-    <t>Hours Constraint</t>
-  </si>
-  <si>
-    <t>Availability Constraint</t>
-  </si>
-  <si>
-    <t>s in S</t>
-  </si>
-  <si>
     <t>c in C</t>
   </si>
   <si>
-    <t>Suppose:</t>
-  </si>
-  <si>
-    <t>s = 2</t>
-  </si>
-  <si>
-    <t>c = MATH2924</t>
-  </si>
-  <si>
     <t>p in P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sched </t>
-  </si>
-  <si>
-    <t>prereq</t>
-  </si>
-  <si>
-    <t>*</t>
-  </si>
-  <si>
-    <t>sched</t>
   </si>
 </sst>
 </file>
@@ -346,7 +301,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -359,28 +314,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -461,7 +401,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -478,32 +418,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -511,7 +433,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -520,8 +442,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -29508,8 +29430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7CDD2E9-B0AB-4B78-AAF0-949DF9D7B865}">
   <dimension ref="A1:AN1004"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -34296,15 +34218,15 @@
     <row r="43" spans="1:39" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
-      <c r="C43" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="D43" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="E43" s="19"/>
-      <c r="F43" s="19"/>
-      <c r="G43" s="20"/>
+      <c r="C43" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="13"/>
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
       <c r="J43" s="3"/>
@@ -34341,7 +34263,7 @@
     <row r="44" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
-      <c r="C44" s="16"/>
+      <c r="C44" s="9"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
@@ -34380,60 +34302,60 @@
       <c r="AM44" s="3"/>
     </row>
     <row r="45" spans="1:39" x14ac:dyDescent="0.45">
-      <c r="C45" s="16"/>
+      <c r="C45" s="9"/>
     </row>
     <row r="46" spans="1:39" x14ac:dyDescent="0.45">
-      <c r="C46" s="16"/>
+      <c r="C46" s="9"/>
     </row>
     <row r="47" spans="1:39" x14ac:dyDescent="0.45">
-      <c r="C47" s="16"/>
+      <c r="C47" s="9"/>
     </row>
     <row r="48" spans="1:39" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C48" s="17"/>
+      <c r="C48" s="10"/>
     </row>
     <row r="50" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="B50" s="9"/>
-      <c r="C50" s="9"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="9"/>
-      <c r="H50" s="9"/>
-      <c r="I50" s="9"/>
-      <c r="J50" s="9"/>
-      <c r="K50" s="9"/>
-      <c r="L50" s="9"/>
-      <c r="M50" s="9"/>
-      <c r="N50" s="9"/>
-      <c r="O50" s="9"/>
-      <c r="P50" s="9"/>
-      <c r="Q50" s="9"/>
-      <c r="R50" s="9"/>
-      <c r="S50" s="9"/>
-      <c r="T50" s="9"/>
-      <c r="U50" s="9"/>
-      <c r="V50" s="9"/>
-      <c r="W50" s="9"/>
-      <c r="X50" s="9"/>
-      <c r="Y50" s="9"/>
-      <c r="Z50" s="9"/>
-      <c r="AA50" s="9"/>
-      <c r="AB50" s="9"/>
-      <c r="AC50" s="9"/>
-      <c r="AD50" s="9"/>
-      <c r="AE50" s="9"/>
-      <c r="AF50" s="9"/>
-      <c r="AG50" s="9"/>
-      <c r="AH50" s="9"/>
-      <c r="AI50" s="9"/>
-      <c r="AJ50" s="9"/>
-      <c r="AK50" s="9"/>
-      <c r="AL50" s="9"/>
-      <c r="AM50" s="9"/>
-      <c r="AN50" s="9"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="7"/>
+      <c r="H50" s="7"/>
+      <c r="I50" s="7"/>
+      <c r="J50" s="7"/>
+      <c r="K50" s="7"/>
+      <c r="L50" s="7"/>
+      <c r="M50" s="7"/>
+      <c r="N50" s="7"/>
+      <c r="O50" s="7"/>
+      <c r="P50" s="7"/>
+      <c r="Q50" s="7"/>
+      <c r="R50" s="7"/>
+      <c r="S50" s="7"/>
+      <c r="T50" s="7"/>
+      <c r="U50" s="7"/>
+      <c r="V50" s="7"/>
+      <c r="W50" s="7"/>
+      <c r="X50" s="7"/>
+      <c r="Y50" s="7"/>
+      <c r="Z50" s="7"/>
+      <c r="AA50" s="7"/>
+      <c r="AB50" s="7"/>
+      <c r="AC50" s="7"/>
+      <c r="AD50" s="7"/>
+      <c r="AE50" s="7"/>
+      <c r="AF50" s="7"/>
+      <c r="AG50" s="7"/>
+      <c r="AH50" s="7"/>
+      <c r="AI50" s="7"/>
+      <c r="AJ50" s="7"/>
+      <c r="AK50" s="7"/>
+      <c r="AL50" s="7"/>
+      <c r="AM50" s="7"/>
+      <c r="AN50" s="7"/>
     </row>
     <row r="51" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A51" s="8"/>
+      <c r="A51" s="6"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
@@ -34475,7 +34397,7 @@
       <c r="AN51" s="3"/>
     </row>
     <row r="52" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A52" s="8"/>
+      <c r="A52" s="6"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
@@ -34517,7 +34439,7 @@
       <c r="AN52" s="3"/>
     </row>
     <row r="53" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A53" s="8"/>
+      <c r="A53" s="6"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
@@ -34559,7 +34481,7 @@
       <c r="AN53" s="3"/>
     </row>
     <row r="54" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A54" s="8"/>
+      <c r="A54" s="6"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
@@ -34601,7 +34523,7 @@
       <c r="AN54" s="3"/>
     </row>
     <row r="55" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A55" s="8"/>
+      <c r="A55" s="6"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
@@ -34643,7 +34565,7 @@
       <c r="AN55" s="3"/>
     </row>
     <row r="56" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A56" s="8"/>
+      <c r="A56" s="6"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
@@ -34685,7 +34607,7 @@
       <c r="AN56" s="3"/>
     </row>
     <row r="57" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A57" s="8"/>
+      <c r="A57" s="6"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
@@ -34727,7 +34649,7 @@
       <c r="AN57" s="3"/>
     </row>
     <row r="58" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A58" s="8"/>
+      <c r="A58" s="6"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
@@ -34769,7 +34691,7 @@
       <c r="AN58" s="3"/>
     </row>
     <row r="59" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A59" s="8"/>
+      <c r="A59" s="6"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
@@ -34811,7 +34733,7 @@
       <c r="AN59" s="3"/>
     </row>
     <row r="60" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A60" s="8"/>
+      <c r="A60" s="6"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
@@ -34853,7 +34775,7 @@
       <c r="AN60" s="3"/>
     </row>
     <row r="61" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A61" s="8"/>
+      <c r="A61" s="6"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
@@ -34894,7 +34816,7 @@
       <c r="AN61" s="3"/>
     </row>
     <row r="62" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A62" s="8"/>
+      <c r="A62" s="6"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
@@ -34936,7 +34858,7 @@
       <c r="AN62" s="3"/>
     </row>
     <row r="63" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A63" s="8"/>
+      <c r="A63" s="6"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
@@ -34978,7 +34900,7 @@
       <c r="AN63" s="3"/>
     </row>
     <row r="64" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A64" s="8"/>
+      <c r="A64" s="6"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
@@ -35020,7 +34942,7 @@
       <c r="AN64" s="3"/>
     </row>
     <row r="65" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A65" s="8"/>
+      <c r="A65" s="6"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
@@ -35062,7 +34984,7 @@
       <c r="AN65" s="3"/>
     </row>
     <row r="66" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A66" s="8"/>
+      <c r="A66" s="6"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
@@ -35104,7 +35026,7 @@
       <c r="AN66" s="3"/>
     </row>
     <row r="67" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A67" s="8"/>
+      <c r="A67" s="6"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
@@ -35146,7 +35068,7 @@
       <c r="AN67" s="3"/>
     </row>
     <row r="68" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A68" s="8"/>
+      <c r="A68" s="6"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
@@ -35188,7 +35110,7 @@
       <c r="AN68" s="3"/>
     </row>
     <row r="69" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A69" s="8"/>
+      <c r="A69" s="6"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
@@ -35230,7 +35152,7 @@
       <c r="AN69" s="3"/>
     </row>
     <row r="70" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A70" s="8"/>
+      <c r="A70" s="6"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
@@ -35272,7 +35194,7 @@
       <c r="AN70" s="3"/>
     </row>
     <row r="71" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A71" s="8"/>
+      <c r="A71" s="6"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
       <c r="D71" s="3"/>
@@ -35314,7 +35236,7 @@
       <c r="AN71" s="3"/>
     </row>
     <row r="72" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A72" s="8"/>
+      <c r="A72" s="6"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
       <c r="D72" s="3"/>
@@ -35356,7 +35278,7 @@
       <c r="AN72" s="3"/>
     </row>
     <row r="73" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A73" s="8"/>
+      <c r="A73" s="6"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
@@ -35398,7 +35320,7 @@
       <c r="AN73" s="3"/>
     </row>
     <row r="74" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A74" s="8"/>
+      <c r="A74" s="6"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
       <c r="D74" s="3"/>
@@ -35440,7 +35362,7 @@
       <c r="AN74" s="3"/>
     </row>
     <row r="75" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A75" s="8"/>
+      <c r="A75" s="6"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
       <c r="D75" s="3"/>
@@ -35482,7 +35404,7 @@
       <c r="AN75" s="3"/>
     </row>
     <row r="76" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A76" s="8"/>
+      <c r="A76" s="6"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
       <c r="D76" s="3"/>
@@ -35524,7 +35446,7 @@
       <c r="AN76" s="3"/>
     </row>
     <row r="77" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A77" s="8"/>
+      <c r="A77" s="6"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
       <c r="D77" s="3"/>
@@ -35566,7 +35488,7 @@
       <c r="AN77" s="3"/>
     </row>
     <row r="78" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A78" s="8"/>
+      <c r="A78" s="6"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
       <c r="D78" s="3"/>
@@ -35608,7 +35530,7 @@
       <c r="AN78" s="3"/>
     </row>
     <row r="79" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A79" s="8"/>
+      <c r="A79" s="6"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
       <c r="D79" s="3"/>
@@ -35650,7 +35572,7 @@
       <c r="AN79" s="3"/>
     </row>
     <row r="80" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A80" s="8"/>
+      <c r="A80" s="6"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
       <c r="D80" s="3"/>
@@ -35692,7 +35614,7 @@
       <c r="AN80" s="3"/>
     </row>
     <row r="81" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A81" s="8"/>
+      <c r="A81" s="6"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
       <c r="D81" s="3"/>
@@ -35734,7 +35656,7 @@
       <c r="AN81" s="3"/>
     </row>
     <row r="82" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A82" s="8"/>
+      <c r="A82" s="6"/>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
       <c r="D82" s="3"/>
@@ -35776,7 +35698,7 @@
       <c r="AN82" s="3"/>
     </row>
     <row r="83" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A83" s="8"/>
+      <c r="A83" s="6"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
       <c r="D83" s="3"/>
@@ -35818,7 +35740,7 @@
       <c r="AN83" s="3"/>
     </row>
     <row r="84" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A84" s="8"/>
+      <c r="A84" s="6"/>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
       <c r="D84" s="3"/>
@@ -35860,7 +35782,7 @@
       <c r="AN84" s="3"/>
     </row>
     <row r="85" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A85" s="8"/>
+      <c r="A85" s="6"/>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
       <c r="D85" s="3"/>
@@ -35902,7 +35824,7 @@
       <c r="AN85" s="3"/>
     </row>
     <row r="86" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A86" s="8"/>
+      <c r="A86" s="6"/>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
       <c r="D86" s="3"/>
@@ -35944,7 +35866,7 @@
       <c r="AN86" s="3"/>
     </row>
     <row r="87" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A87" s="8"/>
+      <c r="A87" s="6"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
       <c r="D87" s="3"/>
@@ -35986,7 +35908,7 @@
       <c r="AN87" s="3"/>
     </row>
     <row r="88" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A88" s="8"/>
+      <c r="A88" s="6"/>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
       <c r="D88" s="3"/>
@@ -36028,7 +35950,7 @@
       <c r="AN88" s="3"/>
     </row>
     <row r="89" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A89" s="8"/>
+      <c r="A89" s="6"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
       <c r="D89" s="3"/>
@@ -73595,10 +73517,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D099514-66A9-40BB-8236-071D2A75DD12}">
-  <dimension ref="A1:Q93"/>
+  <dimension ref="A1:Q97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView zoomScale="83" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -73637,6 +73559,12 @@
       <c r="I1" s="3" t="s">
         <v>62</v>
       </c>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
@@ -73654,8 +73582,12 @@
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
@@ -73673,6 +73605,12 @@
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
@@ -73690,17 +73628,14 @@
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
-      <c r="M4" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -73716,8 +73651,14 @@
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
-    </row>
-    <row r="6" spans="1:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
@@ -73733,15 +73674,14 @@
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
-      <c r="M6" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="14"/>
-    </row>
-    <row r="7" spans="1:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
@@ -73757,15 +73697,12 @@
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
-      <c r="M7" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="N7" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="14"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
@@ -73783,7 +73720,12 @@
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
-      <c r="M8" s="16"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
@@ -73801,7 +73743,12 @@
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
-      <c r="M9" s="16"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
@@ -73819,7 +73766,12 @@
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
-      <c r="M10" s="16"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
@@ -73837,9 +73789,14 @@
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
-      <c r="M11" s="16"/>
-    </row>
-    <row r="12" spans="1:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
         <v>20</v>
       </c>
@@ -73855,7 +73812,12 @@
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
-      <c r="M12" s="17"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
@@ -73873,6 +73835,12 @@
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
@@ -73890,6 +73858,12 @@
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
@@ -73907,6 +73881,12 @@
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
@@ -73924,6 +73904,12 @@
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
@@ -73941,6 +73927,12 @@
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
@@ -73958,6 +73950,12 @@
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
@@ -74026,21 +74024,6 @@
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
-      <c r="M22" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="N22" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="O22" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="P22" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q22" s="4" t="s">
-        <v>79</v>
-      </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
@@ -74331,1852 +74314,63 @@
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A43" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="B43" s="10"/>
-      <c r="C43" s="10"/>
-      <c r="D43" s="10"/>
-      <c r="E43" s="10"/>
-      <c r="F43" s="10"/>
-      <c r="G43" s="10"/>
-      <c r="H43" s="10"/>
-      <c r="I43" s="10"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A44" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B44" s="6">
-        <v>12</v>
-      </c>
-      <c r="C44" s="6">
-        <v>12</v>
-      </c>
-      <c r="D44" s="6">
-        <v>12</v>
-      </c>
-      <c r="E44" s="6">
-        <v>12</v>
-      </c>
-      <c r="F44" s="6">
-        <v>12</v>
-      </c>
-      <c r="G44" s="6">
-        <v>12</v>
-      </c>
-      <c r="H44" s="6">
-        <v>12</v>
-      </c>
-      <c r="I44" s="6">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="B45" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="F45" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="G45" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="H45" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="I45" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A46" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B46" s="4">
-        <f t="shared" ref="B46:I46" si="0">SUM(B2:B39)</f>
-        <v>6</v>
-      </c>
-      <c r="C46" s="4">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="D46" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E46" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F46" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G46" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H46" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I46" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="B47" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F47" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="G47" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="H47" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="I47" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A48" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B48" s="6">
-        <v>20</v>
-      </c>
-      <c r="C48" s="6">
-        <v>20</v>
-      </c>
-      <c r="D48" s="6">
-        <v>20</v>
-      </c>
-      <c r="E48" s="6">
-        <v>20</v>
-      </c>
-      <c r="F48" s="6">
-        <v>20</v>
-      </c>
-      <c r="G48" s="6">
-        <v>20</v>
-      </c>
-      <c r="H48" s="6">
-        <v>20</v>
-      </c>
-      <c r="I48" s="6">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A54" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="B54" s="10"/>
-      <c r="C54" s="10"/>
-      <c r="D54" s="10"/>
-      <c r="E54" s="10"/>
-      <c r="F54" s="10"/>
-      <c r="G54" s="10"/>
-      <c r="H54" s="10"/>
-      <c r="I54" s="10"/>
-      <c r="J54" s="10"/>
-      <c r="K54" s="10"/>
-    </row>
-    <row r="55" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A55" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F55" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G55" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="H55" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="I55" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A56" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B56" s="3">
-        <f>B2*'ISE Availability'!B2</f>
-        <v>0</v>
-      </c>
-      <c r="C56" s="3">
-        <f>C2*'ISE Availability'!C2</f>
-        <v>0</v>
-      </c>
-      <c r="D56" s="3">
-        <f>D2*'ISE Availability'!D2</f>
-        <v>0</v>
-      </c>
-      <c r="E56" s="3">
-        <f>E2*'ISE Availability'!E2</f>
-        <v>0</v>
-      </c>
-      <c r="F56" s="3">
-        <f>F2*'ISE Availability'!F2</f>
-        <v>0</v>
-      </c>
-      <c r="G56" s="3">
-        <f>G2*'ISE Availability'!G2</f>
-        <v>0</v>
-      </c>
-      <c r="H56" s="3">
-        <f>H2*'ISE Availability'!H2</f>
-        <v>0</v>
-      </c>
-      <c r="I56" s="3">
-        <f>I2*'ISE Availability'!I2</f>
-        <v>0</v>
-      </c>
-      <c r="J56" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="K56" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A57" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B57" s="3">
-        <f>B3*'ISE Availability'!B3</f>
-        <v>0</v>
-      </c>
-      <c r="C57" s="3">
-        <f>C3*'ISE Availability'!C3</f>
-        <v>0</v>
-      </c>
-      <c r="D57" s="3">
-        <f>D3*'ISE Availability'!D3</f>
-        <v>0</v>
-      </c>
-      <c r="E57" s="3">
-        <f>E3*'ISE Availability'!E3</f>
-        <v>0</v>
-      </c>
-      <c r="F57" s="3">
-        <f>F3*'ISE Availability'!F3</f>
-        <v>0</v>
-      </c>
-      <c r="G57" s="3">
-        <f>G3*'ISE Availability'!G3</f>
-        <v>0</v>
-      </c>
-      <c r="H57" s="3">
-        <f>H3*'ISE Availability'!H3</f>
-        <v>0</v>
-      </c>
-      <c r="I57" s="3">
-        <f>I3*'ISE Availability'!I3</f>
-        <v>0</v>
-      </c>
-      <c r="J57" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="K57" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A58" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B58" s="3">
-        <f>B4*'ISE Availability'!B4</f>
-        <v>1</v>
-      </c>
-      <c r="C58" s="3">
-        <f>C4*'ISE Availability'!C4</f>
-        <v>0</v>
-      </c>
-      <c r="D58" s="3">
-        <f>D4*'ISE Availability'!D4</f>
-        <v>0</v>
-      </c>
-      <c r="E58" s="3">
-        <f>E4*'ISE Availability'!E4</f>
-        <v>0</v>
-      </c>
-      <c r="F58" s="3">
-        <f>F4*'ISE Availability'!F4</f>
-        <v>0</v>
-      </c>
-      <c r="G58" s="3">
-        <f>G4*'ISE Availability'!G4</f>
-        <v>0</v>
-      </c>
-      <c r="H58" s="3">
-        <f>H4*'ISE Availability'!H4</f>
-        <v>0</v>
-      </c>
-      <c r="I58" s="3">
-        <f>I4*'ISE Availability'!I4</f>
-        <v>0</v>
-      </c>
-      <c r="J58" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="K58" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A59" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B59" s="3">
-        <f>B5*'ISE Availability'!B5</f>
-        <v>0</v>
-      </c>
-      <c r="C59" s="3">
-        <f>C5*'ISE Availability'!C5</f>
-        <v>0</v>
-      </c>
-      <c r="D59" s="3">
-        <f>D5*'ISE Availability'!D5</f>
-        <v>0</v>
-      </c>
-      <c r="E59" s="3">
-        <f>E5*'ISE Availability'!E5</f>
-        <v>0</v>
-      </c>
-      <c r="F59" s="3">
-        <f>F5*'ISE Availability'!F5</f>
-        <v>0</v>
-      </c>
-      <c r="G59" s="3">
-        <f>G5*'ISE Availability'!G5</f>
-        <v>0</v>
-      </c>
-      <c r="H59" s="3">
-        <f>H5*'ISE Availability'!H5</f>
-        <v>0</v>
-      </c>
-      <c r="I59" s="3">
-        <f>I5*'ISE Availability'!I5</f>
-        <v>0</v>
-      </c>
-      <c r="J59" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="K59" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A60" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B60" s="3">
-        <f>B6*'ISE Availability'!B6</f>
-        <v>0</v>
-      </c>
-      <c r="C60" s="3">
-        <f>C6*'ISE Availability'!C6</f>
-        <v>0</v>
-      </c>
-      <c r="D60" s="3">
-        <f>D6*'ISE Availability'!D6</f>
-        <v>0</v>
-      </c>
-      <c r="E60" s="3">
-        <f>E6*'ISE Availability'!E6</f>
-        <v>0</v>
-      </c>
-      <c r="F60" s="3">
-        <f>F6*'ISE Availability'!F6</f>
-        <v>0</v>
-      </c>
-      <c r="G60" s="3">
-        <f>G6*'ISE Availability'!G6</f>
-        <v>0</v>
-      </c>
-      <c r="H60" s="3">
-        <f>H6*'ISE Availability'!H6</f>
-        <v>0</v>
-      </c>
-      <c r="I60" s="3">
-        <f>I6*'ISE Availability'!I6</f>
-        <v>0</v>
-      </c>
-      <c r="J60" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="K60" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A61" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B61" s="3">
-        <f>B7*'ISE Availability'!B7</f>
-        <v>0</v>
-      </c>
-      <c r="C61" s="3">
-        <f>C7*'ISE Availability'!C7</f>
-        <v>0</v>
-      </c>
-      <c r="D61" s="3">
-        <f>D7*'ISE Availability'!D7</f>
-        <v>0</v>
-      </c>
-      <c r="E61" s="3">
-        <f>E7*'ISE Availability'!E7</f>
-        <v>0</v>
-      </c>
-      <c r="F61" s="3">
-        <f>F7*'ISE Availability'!F7</f>
-        <v>0</v>
-      </c>
-      <c r="G61" s="3">
-        <f>G7*'ISE Availability'!G7</f>
-        <v>0</v>
-      </c>
-      <c r="H61" s="3">
-        <f>H7*'ISE Availability'!H7</f>
-        <v>0</v>
-      </c>
-      <c r="I61" s="3">
-        <f>I7*'ISE Availability'!I7</f>
-        <v>0</v>
-      </c>
-      <c r="J61" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="K61" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A62" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B62" s="3">
-        <f>B8*'ISE Availability'!B8</f>
-        <v>0</v>
-      </c>
-      <c r="C62" s="3">
-        <f>C8*'ISE Availability'!C8</f>
-        <v>1</v>
-      </c>
-      <c r="D62" s="3">
-        <f>D8*'ISE Availability'!D8</f>
-        <v>0</v>
-      </c>
-      <c r="E62" s="3">
-        <f>E8*'ISE Availability'!E8</f>
-        <v>0</v>
-      </c>
-      <c r="F62" s="3">
-        <f>F8*'ISE Availability'!F8</f>
-        <v>0</v>
-      </c>
-      <c r="G62" s="3">
-        <f>G8*'ISE Availability'!G8</f>
-        <v>0</v>
-      </c>
-      <c r="H62" s="3">
-        <f>H8*'ISE Availability'!H8</f>
-        <v>0</v>
-      </c>
-      <c r="I62" s="3">
-        <f>I8*'ISE Availability'!I8</f>
-        <v>0</v>
-      </c>
-      <c r="J62" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="K62" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A63" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B63" s="3">
-        <f>B9*'ISE Availability'!B9</f>
-        <v>0</v>
-      </c>
-      <c r="C63" s="3">
-        <f>C9*'ISE Availability'!C9</f>
-        <v>1</v>
-      </c>
-      <c r="D63" s="3">
-        <f>D9*'ISE Availability'!D9</f>
-        <v>0</v>
-      </c>
-      <c r="E63" s="3">
-        <f>E9*'ISE Availability'!E9</f>
-        <v>0</v>
-      </c>
-      <c r="F63" s="3">
-        <f>F9*'ISE Availability'!F9</f>
-        <v>0</v>
-      </c>
-      <c r="G63" s="3">
-        <f>G9*'ISE Availability'!G9</f>
-        <v>0</v>
-      </c>
-      <c r="H63" s="3">
-        <f>H9*'ISE Availability'!H9</f>
-        <v>0</v>
-      </c>
-      <c r="I63" s="3">
-        <f>I9*'ISE Availability'!I9</f>
-        <v>0</v>
-      </c>
-      <c r="J63" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="K63" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A64" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B64" s="3">
-        <f>B10*'ISE Availability'!B10</f>
-        <v>0</v>
-      </c>
-      <c r="C64" s="3">
-        <f>C10*'ISE Availability'!C10</f>
-        <v>0</v>
-      </c>
-      <c r="D64" s="3">
-        <f>D10*'ISE Availability'!D10</f>
-        <v>0</v>
-      </c>
-      <c r="E64" s="3">
-        <f>E10*'ISE Availability'!E10</f>
-        <v>0</v>
-      </c>
-      <c r="F64" s="3">
-        <f>F10*'ISE Availability'!F10</f>
-        <v>0</v>
-      </c>
-      <c r="G64" s="3">
-        <f>G10*'ISE Availability'!G10</f>
-        <v>0</v>
-      </c>
-      <c r="H64" s="3">
-        <f>H10*'ISE Availability'!H10</f>
-        <v>0</v>
-      </c>
-      <c r="I64" s="3">
-        <f>I10*'ISE Availability'!I10</f>
-        <v>0</v>
-      </c>
-      <c r="J64" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="K64" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A65" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B65" s="3">
-        <f>B11*'ISE Availability'!B11</f>
-        <v>0</v>
-      </c>
-      <c r="C65" s="3">
-        <f>C11*'ISE Availability'!C11</f>
-        <v>0</v>
-      </c>
-      <c r="D65" s="3">
-        <f>D11*'ISE Availability'!D11</f>
-        <v>0</v>
-      </c>
-      <c r="E65" s="3">
-        <f>E11*'ISE Availability'!E11</f>
-        <v>0</v>
-      </c>
-      <c r="F65" s="3">
-        <f>F11*'ISE Availability'!F11</f>
-        <v>0</v>
-      </c>
-      <c r="G65" s="3">
-        <f>G11*'ISE Availability'!G11</f>
-        <v>0</v>
-      </c>
-      <c r="H65" s="3">
-        <f>H11*'ISE Availability'!H11</f>
-        <v>0</v>
-      </c>
-      <c r="I65" s="3">
-        <f>I11*'ISE Availability'!I11</f>
-        <v>0</v>
-      </c>
-      <c r="J65" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="K65" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A66" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B66" s="3">
-        <f>B12*'ISE Availability'!B12</f>
-        <v>0</v>
-      </c>
-      <c r="C66" s="3">
-        <f>C12*'ISE Availability'!C12</f>
-        <v>0</v>
-      </c>
-      <c r="D66" s="3">
-        <f>D12*'ISE Availability'!D12</f>
-        <v>0</v>
-      </c>
-      <c r="E66" s="3">
-        <f>E12*'ISE Availability'!E12</f>
-        <v>0</v>
-      </c>
-      <c r="F66" s="3">
-        <f>F12*'ISE Availability'!F12</f>
-        <v>0</v>
-      </c>
-      <c r="G66" s="3">
-        <f>G12*'ISE Availability'!G12</f>
-        <v>0</v>
-      </c>
-      <c r="H66" s="3">
-        <f>H12*'ISE Availability'!H12</f>
-        <v>0</v>
-      </c>
-      <c r="I66" s="3">
-        <f>I12*'ISE Availability'!I12</f>
-        <v>0</v>
-      </c>
-      <c r="J66" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="K66" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A67" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B67" s="3">
-        <f>B13*'ISE Availability'!B13</f>
-        <v>1</v>
-      </c>
-      <c r="C67" s="3">
-        <f>C13*'ISE Availability'!C13</f>
-        <v>0</v>
-      </c>
-      <c r="D67" s="3">
-        <f>D13*'ISE Availability'!D13</f>
-        <v>0</v>
-      </c>
-      <c r="E67" s="3">
-        <f>E13*'ISE Availability'!E13</f>
-        <v>0</v>
-      </c>
-      <c r="F67" s="3">
-        <f>F13*'ISE Availability'!F13</f>
-        <v>0</v>
-      </c>
-      <c r="G67" s="3">
-        <f>G13*'ISE Availability'!G13</f>
-        <v>0</v>
-      </c>
-      <c r="H67" s="3">
-        <f>H13*'ISE Availability'!H13</f>
-        <v>0</v>
-      </c>
-      <c r="I67" s="3">
-        <f>I13*'ISE Availability'!I13</f>
-        <v>0</v>
-      </c>
-      <c r="J67" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="K67" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A68" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B68" s="3">
-        <f>B14*'ISE Availability'!B14</f>
-        <v>0</v>
-      </c>
-      <c r="C68" s="3">
-        <f>C14*'ISE Availability'!C14</f>
-        <v>1</v>
-      </c>
-      <c r="D68" s="3">
-        <f>D14*'ISE Availability'!D14</f>
-        <v>0</v>
-      </c>
-      <c r="E68" s="3">
-        <f>E14*'ISE Availability'!E14</f>
-        <v>0</v>
-      </c>
-      <c r="F68" s="3">
-        <f>F14*'ISE Availability'!F14</f>
-        <v>0</v>
-      </c>
-      <c r="G68" s="3">
-        <f>G14*'ISE Availability'!G14</f>
-        <v>0</v>
-      </c>
-      <c r="H68" s="3">
-        <f>H14*'ISE Availability'!H14</f>
-        <v>0</v>
-      </c>
-      <c r="I68" s="3">
-        <f>I14*'ISE Availability'!I14</f>
-        <v>0</v>
-      </c>
-      <c r="J68" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="K68" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A69" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B69" s="3">
-        <f>B15*'ISE Availability'!B15</f>
-        <v>0</v>
-      </c>
-      <c r="C69" s="3">
-        <f>C15*'ISE Availability'!C15</f>
-        <v>0</v>
-      </c>
-      <c r="D69" s="3">
-        <f>D15*'ISE Availability'!D15</f>
-        <v>0</v>
-      </c>
-      <c r="E69" s="3">
-        <f>E15*'ISE Availability'!E15</f>
-        <v>0</v>
-      </c>
-      <c r="F69" s="3">
-        <f>F15*'ISE Availability'!F15</f>
-        <v>0</v>
-      </c>
-      <c r="G69" s="3">
-        <f>G15*'ISE Availability'!G15</f>
-        <v>0</v>
-      </c>
-      <c r="H69" s="3">
-        <f>H15*'ISE Availability'!H15</f>
-        <v>0</v>
-      </c>
-      <c r="I69" s="3">
-        <f>I15*'ISE Availability'!I15</f>
-        <v>0</v>
-      </c>
-      <c r="J69" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="K69" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A70" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B70" s="3">
-        <f>B16*'ISE Availability'!B16</f>
-        <v>0</v>
-      </c>
-      <c r="C70" s="3">
-        <f>C16*'ISE Availability'!C16</f>
-        <v>0</v>
-      </c>
-      <c r="D70" s="3">
-        <f>D16*'ISE Availability'!D16</f>
-        <v>0</v>
-      </c>
-      <c r="E70" s="3">
-        <f>E16*'ISE Availability'!E16</f>
-        <v>0</v>
-      </c>
-      <c r="F70" s="3">
-        <f>F16*'ISE Availability'!F16</f>
-        <v>0</v>
-      </c>
-      <c r="G70" s="3">
-        <f>G16*'ISE Availability'!G16</f>
-        <v>0</v>
-      </c>
-      <c r="H70" s="3">
-        <f>H16*'ISE Availability'!H16</f>
-        <v>0</v>
-      </c>
-      <c r="I70" s="3">
-        <f>I16*'ISE Availability'!I16</f>
-        <v>0</v>
-      </c>
-      <c r="J70" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="K70" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A71" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B71" s="3">
-        <f>B17*'ISE Availability'!B17</f>
-        <v>0</v>
-      </c>
-      <c r="C71" s="3">
-        <f>C17*'ISE Availability'!C17</f>
-        <v>0</v>
-      </c>
-      <c r="D71" s="3">
-        <f>D17*'ISE Availability'!D17</f>
-        <v>0</v>
-      </c>
-      <c r="E71" s="3">
-        <f>E17*'ISE Availability'!E17</f>
-        <v>0</v>
-      </c>
-      <c r="F71" s="3">
-        <f>F17*'ISE Availability'!F17</f>
-        <v>0</v>
-      </c>
-      <c r="G71" s="3">
-        <f>G17*'ISE Availability'!G17</f>
-        <v>0</v>
-      </c>
-      <c r="H71" s="3">
-        <f>H17*'ISE Availability'!H17</f>
-        <v>0</v>
-      </c>
-      <c r="I71" s="3">
-        <f>I17*'ISE Availability'!I17</f>
-        <v>0</v>
-      </c>
-      <c r="J71" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="K71" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A72" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B72" s="3">
-        <f>B18*'ISE Availability'!B18</f>
-        <v>1</v>
-      </c>
-      <c r="C72" s="3">
-        <f>C18*'ISE Availability'!C18</f>
-        <v>0</v>
-      </c>
-      <c r="D72" s="3">
-        <f>D18*'ISE Availability'!D18</f>
-        <v>0</v>
-      </c>
-      <c r="E72" s="3">
-        <f>E18*'ISE Availability'!E18</f>
-        <v>0</v>
-      </c>
-      <c r="F72" s="3">
-        <f>F18*'ISE Availability'!F18</f>
-        <v>0</v>
-      </c>
-      <c r="G72" s="3">
-        <f>G18*'ISE Availability'!G18</f>
-        <v>0</v>
-      </c>
-      <c r="H72" s="3">
-        <f>H18*'ISE Availability'!H18</f>
-        <v>0</v>
-      </c>
-      <c r="I72" s="3">
-        <f>I18*'ISE Availability'!I18</f>
-        <v>0</v>
-      </c>
-      <c r="J72" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="K72" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A73" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B73" s="3">
-        <f>B19*'ISE Availability'!B19</f>
-        <v>0</v>
-      </c>
-      <c r="C73" s="3">
-        <f>C19*'ISE Availability'!C19</f>
-        <v>0</v>
-      </c>
-      <c r="D73" s="3">
-        <f>D19*'ISE Availability'!D19</f>
-        <v>0</v>
-      </c>
-      <c r="E73" s="3">
-        <f>E19*'ISE Availability'!E19</f>
-        <v>0</v>
-      </c>
-      <c r="F73" s="3">
-        <f>F19*'ISE Availability'!F19</f>
-        <v>0</v>
-      </c>
-      <c r="G73" s="3">
-        <f>G19*'ISE Availability'!G19</f>
-        <v>0</v>
-      </c>
-      <c r="H73" s="3">
-        <f>H19*'ISE Availability'!H19</f>
-        <v>0</v>
-      </c>
-      <c r="I73" s="3">
-        <f>I19*'ISE Availability'!I19</f>
-        <v>0</v>
-      </c>
-      <c r="J73" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="K73" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A74" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B74" s="3">
-        <f>B20*'ISE Availability'!B20</f>
-        <v>0</v>
-      </c>
-      <c r="C74" s="3">
-        <f>C20*'ISE Availability'!C20</f>
-        <v>0</v>
-      </c>
-      <c r="D74" s="3">
-        <f>D20*'ISE Availability'!D20</f>
-        <v>0</v>
-      </c>
-      <c r="E74" s="3">
-        <f>E20*'ISE Availability'!E20</f>
-        <v>0</v>
-      </c>
-      <c r="F74" s="3">
-        <f>F20*'ISE Availability'!F20</f>
-        <v>0</v>
-      </c>
-      <c r="G74" s="3">
-        <f>G20*'ISE Availability'!G20</f>
-        <v>0</v>
-      </c>
-      <c r="H74" s="3">
-        <f>H20*'ISE Availability'!H20</f>
-        <v>0</v>
-      </c>
-      <c r="I74" s="3">
-        <f>I20*'ISE Availability'!I20</f>
-        <v>0</v>
-      </c>
-      <c r="J74" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="K74" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A75" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B75" s="3">
-        <f>B21*'ISE Availability'!B21</f>
-        <v>1</v>
-      </c>
-      <c r="C75" s="3">
-        <f>C21*'ISE Availability'!C21</f>
-        <v>0</v>
-      </c>
-      <c r="D75" s="3">
-        <f>D21*'ISE Availability'!D21</f>
-        <v>0</v>
-      </c>
-      <c r="E75" s="3">
-        <f>E21*'ISE Availability'!E21</f>
-        <v>0</v>
-      </c>
-      <c r="F75" s="3">
-        <f>F21*'ISE Availability'!F21</f>
-        <v>0</v>
-      </c>
-      <c r="G75" s="3">
-        <f>G21*'ISE Availability'!G21</f>
-        <v>0</v>
-      </c>
-      <c r="H75" s="3">
-        <f>H21*'ISE Availability'!H21</f>
-        <v>0</v>
-      </c>
-      <c r="I75" s="3">
-        <f>I21*'ISE Availability'!I21</f>
-        <v>0</v>
-      </c>
-      <c r="J75" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="K75" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A76" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B76" s="3">
-        <f>B22*'ISE Availability'!B22</f>
-        <v>0</v>
-      </c>
-      <c r="C76" s="3">
-        <f>C22*'ISE Availability'!C22</f>
-        <v>0</v>
-      </c>
-      <c r="D76" s="3">
-        <f>D22*'ISE Availability'!D22</f>
-        <v>0</v>
-      </c>
-      <c r="E76" s="3">
-        <f>E22*'ISE Availability'!E22</f>
-        <v>0</v>
-      </c>
-      <c r="F76" s="3">
-        <f>F22*'ISE Availability'!F22</f>
-        <v>0</v>
-      </c>
-      <c r="G76" s="3">
-        <f>G22*'ISE Availability'!G22</f>
-        <v>0</v>
-      </c>
-      <c r="H76" s="3">
-        <f>H22*'ISE Availability'!H22</f>
-        <v>0</v>
-      </c>
-      <c r="I76" s="3">
-        <f>I22*'ISE Availability'!I22</f>
-        <v>0</v>
-      </c>
-      <c r="J76" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="K76" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A77" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B77" s="3">
-        <f>B23*'ISE Availability'!B23</f>
-        <v>0</v>
-      </c>
-      <c r="C77" s="3">
-        <f>C23*'ISE Availability'!C23</f>
-        <v>1</v>
-      </c>
-      <c r="D77" s="3">
-        <f>D23*'ISE Availability'!D23</f>
-        <v>0</v>
-      </c>
-      <c r="E77" s="3">
-        <f>E23*'ISE Availability'!E23</f>
-        <v>0</v>
-      </c>
-      <c r="F77" s="3">
-        <f>F23*'ISE Availability'!F23</f>
-        <v>0</v>
-      </c>
-      <c r="G77" s="3">
-        <f>G23*'ISE Availability'!G23</f>
-        <v>0</v>
-      </c>
-      <c r="H77" s="3">
-        <f>H23*'ISE Availability'!H23</f>
-        <v>0</v>
-      </c>
-      <c r="I77" s="3">
-        <f>I23*'ISE Availability'!I23</f>
-        <v>0</v>
-      </c>
-      <c r="J77" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="K77" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A78" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B78" s="3">
-        <f>B24*'ISE Availability'!B24</f>
-        <v>0</v>
-      </c>
-      <c r="C78" s="3">
-        <f>C24*'ISE Availability'!C24</f>
-        <v>1</v>
-      </c>
-      <c r="D78" s="3">
-        <f>D24*'ISE Availability'!D24</f>
-        <v>0</v>
-      </c>
-      <c r="E78" s="3">
-        <f>E24*'ISE Availability'!E24</f>
-        <v>0</v>
-      </c>
-      <c r="F78" s="3">
-        <f>F24*'ISE Availability'!F24</f>
-        <v>0</v>
-      </c>
-      <c r="G78" s="3">
-        <f>G24*'ISE Availability'!G24</f>
-        <v>0</v>
-      </c>
-      <c r="H78" s="3">
-        <f>H24*'ISE Availability'!H24</f>
-        <v>0</v>
-      </c>
-      <c r="I78" s="3">
-        <f>I24*'ISE Availability'!I24</f>
-        <v>0</v>
-      </c>
-      <c r="J78" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="K78" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A79" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B79" s="3">
-        <f>B25*'ISE Availability'!B25</f>
-        <v>1</v>
-      </c>
-      <c r="C79" s="3">
-        <f>C25*'ISE Availability'!C25</f>
-        <v>0</v>
-      </c>
-      <c r="D79" s="3">
-        <f>D25*'ISE Availability'!D25</f>
-        <v>0</v>
-      </c>
-      <c r="E79" s="3">
-        <f>E25*'ISE Availability'!E25</f>
-        <v>0</v>
-      </c>
-      <c r="F79" s="3">
-        <f>F25*'ISE Availability'!F25</f>
-        <v>0</v>
-      </c>
-      <c r="G79" s="3">
-        <f>G25*'ISE Availability'!G25</f>
-        <v>0</v>
-      </c>
-      <c r="H79" s="3">
-        <f>H25*'ISE Availability'!H25</f>
-        <v>0</v>
-      </c>
-      <c r="I79" s="3">
-        <f>I25*'ISE Availability'!I25</f>
-        <v>0</v>
-      </c>
-      <c r="J79" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="K79" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A80" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B80" s="3">
-        <f>B26*'ISE Availability'!B26</f>
-        <v>0</v>
-      </c>
-      <c r="C80" s="3">
-        <f>C26*'ISE Availability'!C26</f>
-        <v>0</v>
-      </c>
-      <c r="D80" s="3">
-        <f>D26*'ISE Availability'!D26</f>
-        <v>0</v>
-      </c>
-      <c r="E80" s="3">
-        <f>E26*'ISE Availability'!E26</f>
-        <v>0</v>
-      </c>
-      <c r="F80" s="3">
-        <f>F26*'ISE Availability'!F26</f>
-        <v>0</v>
-      </c>
-      <c r="G80" s="3">
-        <f>G26*'ISE Availability'!G26</f>
-        <v>0</v>
-      </c>
-      <c r="H80" s="3">
-        <f>H26*'ISE Availability'!H26</f>
-        <v>0</v>
-      </c>
-      <c r="I80" s="3">
-        <f>I26*'ISE Availability'!I26</f>
-        <v>0</v>
-      </c>
-      <c r="J80" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="K80" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A81" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B81" s="3">
-        <f>B27*'ISE Availability'!B27</f>
-        <v>0</v>
-      </c>
-      <c r="C81" s="3">
-        <f>C27*'ISE Availability'!C27</f>
-        <v>0</v>
-      </c>
-      <c r="D81" s="3">
-        <f>D27*'ISE Availability'!D27</f>
-        <v>0</v>
-      </c>
-      <c r="E81" s="3">
-        <f>E27*'ISE Availability'!E27</f>
-        <v>0</v>
-      </c>
-      <c r="F81" s="3">
-        <f>F27*'ISE Availability'!F27</f>
-        <v>0</v>
-      </c>
-      <c r="G81" s="3">
-        <f>G27*'ISE Availability'!G27</f>
-        <v>0</v>
-      </c>
-      <c r="H81" s="3">
-        <f>H27*'ISE Availability'!H27</f>
-        <v>0</v>
-      </c>
-      <c r="I81" s="3">
-        <f>I27*'ISE Availability'!I27</f>
-        <v>0</v>
-      </c>
-      <c r="J81" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="K81" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A82" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B82" s="3">
-        <f>B28*'ISE Availability'!B28</f>
-        <v>0</v>
-      </c>
-      <c r="C82" s="3">
-        <f>C28*'ISE Availability'!C28</f>
-        <v>0</v>
-      </c>
-      <c r="D82" s="3">
-        <f>D28*'ISE Availability'!D28</f>
-        <v>0</v>
-      </c>
-      <c r="E82" s="3">
-        <f>E28*'ISE Availability'!E28</f>
-        <v>0</v>
-      </c>
-      <c r="F82" s="3">
-        <f>F28*'ISE Availability'!F28</f>
-        <v>0</v>
-      </c>
-      <c r="G82" s="3">
-        <f>G28*'ISE Availability'!G28</f>
-        <v>0</v>
-      </c>
-      <c r="H82" s="3">
-        <f>H28*'ISE Availability'!H28</f>
-        <v>0</v>
-      </c>
-      <c r="I82" s="3">
-        <f>I28*'ISE Availability'!I28</f>
-        <v>0</v>
-      </c>
-      <c r="J82" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="K82" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A83" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B83" s="3">
-        <f>B29*'ISE Availability'!B29</f>
-        <v>0</v>
-      </c>
-      <c r="C83" s="3">
-        <f>C29*'ISE Availability'!C29</f>
-        <v>0</v>
-      </c>
-      <c r="D83" s="3">
-        <f>D29*'ISE Availability'!D29</f>
-        <v>0</v>
-      </c>
-      <c r="E83" s="3">
-        <f>E29*'ISE Availability'!E29</f>
-        <v>0</v>
-      </c>
-      <c r="F83" s="3">
-        <f>F29*'ISE Availability'!F29</f>
-        <v>0</v>
-      </c>
-      <c r="G83" s="3">
-        <f>G29*'ISE Availability'!G29</f>
-        <v>0</v>
-      </c>
-      <c r="H83" s="3">
-        <f>H29*'ISE Availability'!H29</f>
-        <v>0</v>
-      </c>
-      <c r="I83" s="3">
-        <f>I29*'ISE Availability'!I29</f>
-        <v>0</v>
-      </c>
-      <c r="J83" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="K83" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A84" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B84" s="3">
-        <f>B30*'ISE Availability'!B30</f>
-        <v>0</v>
-      </c>
-      <c r="C84" s="3">
-        <f>C30*'ISE Availability'!C30</f>
-        <v>0</v>
-      </c>
-      <c r="D84" s="3">
-        <f>D30*'ISE Availability'!D30</f>
-        <v>0</v>
-      </c>
-      <c r="E84" s="3">
-        <f>E30*'ISE Availability'!E30</f>
-        <v>0</v>
-      </c>
-      <c r="F84" s="3">
-        <f>F30*'ISE Availability'!F30</f>
-        <v>0</v>
-      </c>
-      <c r="G84" s="3">
-        <f>G30*'ISE Availability'!G30</f>
-        <v>0</v>
-      </c>
-      <c r="H84" s="3">
-        <f>H30*'ISE Availability'!H30</f>
-        <v>0</v>
-      </c>
-      <c r="I84" s="3">
-        <f>I30*'ISE Availability'!I30</f>
-        <v>0</v>
-      </c>
-      <c r="J84" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="K84" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A85" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B85" s="3">
-        <f>B31*'ISE Availability'!B31</f>
-        <v>0</v>
-      </c>
-      <c r="C85" s="3">
-        <f>C31*'ISE Availability'!C31</f>
-        <v>0</v>
-      </c>
-      <c r="D85" s="3">
-        <f>D31*'ISE Availability'!D31</f>
-        <v>0</v>
-      </c>
-      <c r="E85" s="3">
-        <f>E31*'ISE Availability'!E31</f>
-        <v>0</v>
-      </c>
-      <c r="F85" s="3">
-        <f>F31*'ISE Availability'!F31</f>
-        <v>0</v>
-      </c>
-      <c r="G85" s="3">
-        <f>G31*'ISE Availability'!G31</f>
-        <v>0</v>
-      </c>
-      <c r="H85" s="3">
-        <f>H31*'ISE Availability'!H31</f>
-        <v>0</v>
-      </c>
-      <c r="I85" s="3">
-        <f>I31*'ISE Availability'!I31</f>
-        <v>0</v>
-      </c>
-      <c r="J85" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="K85" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A86" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B86" s="3">
-        <f>B32*'ISE Availability'!B32</f>
-        <v>0</v>
-      </c>
-      <c r="C86" s="3">
-        <f>C32*'ISE Availability'!C32</f>
-        <v>0</v>
-      </c>
-      <c r="D86" s="3">
-        <f>D32*'ISE Availability'!D32</f>
-        <v>0</v>
-      </c>
-      <c r="E86" s="3">
-        <f>E32*'ISE Availability'!E32</f>
-        <v>0</v>
-      </c>
-      <c r="F86" s="3">
-        <f>F32*'ISE Availability'!F32</f>
-        <v>0</v>
-      </c>
-      <c r="G86" s="3">
-        <f>G32*'ISE Availability'!G32</f>
-        <v>0</v>
-      </c>
-      <c r="H86" s="3">
-        <f>H32*'ISE Availability'!H32</f>
-        <v>0</v>
-      </c>
-      <c r="I86" s="3">
-        <f>I32*'ISE Availability'!I32</f>
-        <v>0</v>
-      </c>
-      <c r="J86" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="K86" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A87" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B87" s="3">
-        <f>B33*'ISE Availability'!B33</f>
-        <v>0</v>
-      </c>
-      <c r="C87" s="3">
-        <f>C33*'ISE Availability'!C33</f>
-        <v>0</v>
-      </c>
-      <c r="D87" s="3">
-        <f>D33*'ISE Availability'!D33</f>
-        <v>0</v>
-      </c>
-      <c r="E87" s="3">
-        <f>E33*'ISE Availability'!E33</f>
-        <v>0</v>
-      </c>
-      <c r="F87" s="3">
-        <f>F33*'ISE Availability'!F33</f>
-        <v>0</v>
-      </c>
-      <c r="G87" s="3">
-        <f>G33*'ISE Availability'!G33</f>
-        <v>0</v>
-      </c>
-      <c r="H87" s="3">
-        <f>H33*'ISE Availability'!H33</f>
-        <v>0</v>
-      </c>
-      <c r="I87" s="3">
-        <f>I33*'ISE Availability'!I33</f>
-        <v>0</v>
-      </c>
-      <c r="J87" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="K87" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A88" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B88" s="3">
-        <f>B34*'ISE Availability'!B34</f>
-        <v>0</v>
-      </c>
-      <c r="C88" s="3">
-        <f>C34*'ISE Availability'!C34</f>
-        <v>0</v>
-      </c>
-      <c r="D88" s="3">
-        <f>D34*'ISE Availability'!D34</f>
-        <v>0</v>
-      </c>
-      <c r="E88" s="3">
-        <f>E34*'ISE Availability'!E34</f>
-        <v>0</v>
-      </c>
-      <c r="F88" s="3">
-        <f>F34*'ISE Availability'!F34</f>
-        <v>0</v>
-      </c>
-      <c r="G88" s="3">
-        <f>G34*'ISE Availability'!G34</f>
-        <v>0</v>
-      </c>
-      <c r="H88" s="3">
-        <f>H34*'ISE Availability'!H34</f>
-        <v>0</v>
-      </c>
-      <c r="I88" s="3">
-        <f>I34*'ISE Availability'!I34</f>
-        <v>0</v>
-      </c>
-      <c r="J88" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="K88" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A89" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B89" s="3">
-        <f>B35*'ISE Availability'!B35</f>
-        <v>0</v>
-      </c>
-      <c r="C89" s="3">
-        <f>C35*'ISE Availability'!C35</f>
-        <v>0</v>
-      </c>
-      <c r="D89" s="3">
-        <f>D35*'ISE Availability'!D35</f>
-        <v>0</v>
-      </c>
-      <c r="E89" s="3">
-        <f>E35*'ISE Availability'!E35</f>
-        <v>0</v>
-      </c>
-      <c r="F89" s="3">
-        <f>F35*'ISE Availability'!F35</f>
-        <v>0</v>
-      </c>
-      <c r="G89" s="3">
-        <f>G35*'ISE Availability'!G35</f>
-        <v>0</v>
-      </c>
-      <c r="H89" s="3">
-        <f>H35*'ISE Availability'!H35</f>
-        <v>0</v>
-      </c>
-      <c r="I89" s="3">
-        <f>I35*'ISE Availability'!I35</f>
-        <v>0</v>
-      </c>
-      <c r="J89" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="K89" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A90" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B90" s="3">
-        <f>B36*'ISE Availability'!B36</f>
-        <v>1</v>
-      </c>
-      <c r="C90" s="3">
-        <f>C36*'ISE Availability'!C36</f>
-        <v>0</v>
-      </c>
-      <c r="D90" s="3">
-        <f>D36*'ISE Availability'!D36</f>
-        <v>0</v>
-      </c>
-      <c r="E90" s="3">
-        <f>E36*'ISE Availability'!E36</f>
-        <v>0</v>
-      </c>
-      <c r="F90" s="3">
-        <f>F36*'ISE Availability'!F36</f>
-        <v>0</v>
-      </c>
-      <c r="G90" s="3">
-        <f>G36*'ISE Availability'!G36</f>
-        <v>0</v>
-      </c>
-      <c r="H90" s="3">
-        <f>H36*'ISE Availability'!H36</f>
-        <v>0</v>
-      </c>
-      <c r="I90" s="3">
-        <f>I36*'ISE Availability'!I36</f>
-        <v>0</v>
-      </c>
-      <c r="J90" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="K90" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A91" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B91" s="3">
-        <f>B37*'ISE Availability'!B37</f>
-        <v>0</v>
-      </c>
-      <c r="C91" s="3">
-        <f>C37*'ISE Availability'!C37</f>
-        <v>0</v>
-      </c>
-      <c r="D91" s="3">
-        <f>D37*'ISE Availability'!D37</f>
-        <v>0</v>
-      </c>
-      <c r="E91" s="3">
-        <f>E37*'ISE Availability'!E37</f>
-        <v>0</v>
-      </c>
-      <c r="F91" s="3">
-        <f>F37*'ISE Availability'!F37</f>
-        <v>0</v>
-      </c>
-      <c r="G91" s="3">
-        <f>G37*'ISE Availability'!G37</f>
-        <v>0</v>
-      </c>
-      <c r="H91" s="3">
-        <f>H37*'ISE Availability'!H37</f>
-        <v>0</v>
-      </c>
-      <c r="I91" s="3">
-        <f>I37*'ISE Availability'!I37</f>
-        <v>0</v>
-      </c>
-      <c r="J91" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="K91" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A92" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B92" s="3">
-        <f>B38*'ISE Availability'!B38</f>
-        <v>0</v>
-      </c>
-      <c r="C92" s="3">
-        <f>C38*'ISE Availability'!C38</f>
-        <v>0</v>
-      </c>
-      <c r="D92" s="3">
-        <f>D38*'ISE Availability'!D38</f>
-        <v>0</v>
-      </c>
-      <c r="E92" s="3">
-        <f>E38*'ISE Availability'!E38</f>
-        <v>0</v>
-      </c>
-      <c r="F92" s="3">
-        <f>F38*'ISE Availability'!F38</f>
-        <v>0</v>
-      </c>
-      <c r="G92" s="3">
-        <f>G38*'ISE Availability'!G38</f>
-        <v>0</v>
-      </c>
-      <c r="H92" s="3">
-        <f>H38*'ISE Availability'!H38</f>
-        <v>0</v>
-      </c>
-      <c r="I92" s="3">
-        <f>I38*'ISE Availability'!I38</f>
-        <v>0</v>
-      </c>
-      <c r="J92" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="K92" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A93" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B93" s="3">
-        <f>B39*'ISE Availability'!B39</f>
-        <v>0</v>
-      </c>
-      <c r="C93" s="3">
-        <f>C39*'ISE Availability'!C39</f>
-        <v>0</v>
-      </c>
-      <c r="D93" s="3">
-        <f>D39*'ISE Availability'!D39</f>
-        <v>0</v>
-      </c>
-      <c r="E93" s="3">
-        <f>E39*'ISE Availability'!E39</f>
-        <v>0</v>
-      </c>
-      <c r="F93" s="3">
-        <f>F39*'ISE Availability'!F39</f>
-        <v>0</v>
-      </c>
-      <c r="G93" s="3">
-        <f>G39*'ISE Availability'!G39</f>
-        <v>0</v>
-      </c>
-      <c r="H93" s="3">
-        <f>H39*'ISE Availability'!H39</f>
-        <v>0</v>
-      </c>
-      <c r="I93" s="3">
-        <f>I39*'ISE Availability'!I39</f>
-        <v>0</v>
-      </c>
-      <c r="J93" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="K93" s="6">
-        <v>1</v>
-      </c>
-    </row>
+    <row r="42" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="43" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="44" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="45" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="46" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="47" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="48" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="49" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="50" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="51" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="52" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="53" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="54" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="55" s="14" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="56" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="57" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="58" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="59" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="60" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="61" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="62" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="63" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="64" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="65" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="66" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="67" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="68" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="69" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="70" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="71" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="72" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="73" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="74" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="75" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="76" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="77" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="78" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="79" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="80" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="81" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="82" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="83" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="84" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="85" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="86" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="87" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="88" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="89" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="90" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="91" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="92" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="93" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="94" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="95" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="96" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="97" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A43:I43"/>
-    <mergeCell ref="A54:K54"/>
-    <mergeCell ref="M6:Q6"/>
-    <mergeCell ref="M7:M12"/>
-    <mergeCell ref="N7:Q7"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Working on extract stage
</commit_message>
<xml_diff>
--- a/Schedule-Data.xlsx
+++ b/Schedule-Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\pipe\Shaman\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{142DBEF8-3542-4D69-9C16-01A115B3F931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5AE4B88-078E-4E83-8CA5-B7BFD3FE471A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" activeTab="2" xr2:uid="{503009C4-0C10-4696-AB1F-D7C487AD1E49}"/>
   </bookViews>
@@ -16,45 +16,46 @@
     <sheet name="ISE" sheetId="1" r:id="rId1"/>
     <sheet name="ISE Availability" sheetId="7" r:id="rId2"/>
     <sheet name="ISE Prereqs" sheetId="6" r:id="rId3"/>
-    <sheet name="Schedule" sheetId="8" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="9" r:id="rId4"/>
+    <sheet name="Schedule" sheetId="8" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="3" hidden="1">Schedule!$B$2:$I$39</definedName>
-    <definedName name="solver_cvg" localSheetId="3" hidden="1">0.0001</definedName>
-    <definedName name="solver_drv" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_eng" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_est" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_itr" localSheetId="3" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="3" hidden="1">Schedule!$B$2:$I$39</definedName>
-    <definedName name="solver_lhs2" localSheetId="3" hidden="1">Schedule!$B$46:$I$46</definedName>
-    <definedName name="solver_lhs3" localSheetId="3" hidden="1">Schedule!$B$46:$I$46</definedName>
-    <definedName name="solver_mip" localSheetId="3" hidden="1">2147483647</definedName>
-    <definedName name="solver_mni" localSheetId="3" hidden="1">30</definedName>
-    <definedName name="solver_mrt" localSheetId="3" hidden="1">0.075</definedName>
-    <definedName name="solver_msl" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_neg" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_nod" localSheetId="3" hidden="1">2147483647</definedName>
-    <definedName name="solver_num" localSheetId="3" hidden="1">3</definedName>
-    <definedName name="solver_nwt" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="3" hidden="1">Schedule!$O$2</definedName>
-    <definedName name="solver_pre" localSheetId="3" hidden="1">0.000001</definedName>
-    <definedName name="solver_rbv" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_rel1" localSheetId="3" hidden="1">5</definedName>
-    <definedName name="solver_rel2" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_rel3" localSheetId="3" hidden="1">3</definedName>
-    <definedName name="solver_rhs1" localSheetId="3" hidden="1">"binary"</definedName>
-    <definedName name="solver_rhs2" localSheetId="3" hidden="1">Schedule!$B$48:$I$48</definedName>
-    <definedName name="solver_rhs3" localSheetId="3" hidden="1">Schedule!$B$44:$I$44</definedName>
-    <definedName name="solver_rlx" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_rsd" localSheetId="3" hidden="1">0</definedName>
-    <definedName name="solver_scl" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_sho" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_ssz" localSheetId="3" hidden="1">100</definedName>
-    <definedName name="solver_tim" localSheetId="3" hidden="1">2147483647</definedName>
-    <definedName name="solver_tol" localSheetId="3" hidden="1">0.01</definedName>
-    <definedName name="solver_typ" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
-    <definedName name="solver_ver" localSheetId="3" hidden="1">3</definedName>
+    <definedName name="solver_adj" localSheetId="4" hidden="1">Schedule!$B$2:$I$39</definedName>
+    <definedName name="solver_cvg" localSheetId="4" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="4" hidden="1">Schedule!$B$2:$I$39</definedName>
+    <definedName name="solver_lhs2" localSheetId="4" hidden="1">Schedule!$B$46:$I$46</definedName>
+    <definedName name="solver_lhs3" localSheetId="4" hidden="1">Schedule!$B$46:$I$46</definedName>
+    <definedName name="solver_mip" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="4" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="4" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="4" hidden="1">3</definedName>
+    <definedName name="solver_nwt" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="4" hidden="1">Schedule!$O$2</definedName>
+    <definedName name="solver_pre" localSheetId="4" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="4" hidden="1">5</definedName>
+    <definedName name="solver_rel2" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_rel3" localSheetId="4" hidden="1">3</definedName>
+    <definedName name="solver_rhs1" localSheetId="4" hidden="1">"binary"</definedName>
+    <definedName name="solver_rhs2" localSheetId="4" hidden="1">Schedule!$B$48:$I$48</definedName>
+    <definedName name="solver_rhs3" localSheetId="4" hidden="1">Schedule!$B$44:$I$44</definedName>
+    <definedName name="solver_rlx" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="4" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="4" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_val" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="4" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -77,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="65">
   <si>
     <t>Fall</t>
   </si>
@@ -401,7 +402,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -441,9 +442,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -761,8 +759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D6FC798-9B17-413F-A36C-134B42F149EF}">
   <dimension ref="A1:Y1004"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView topLeftCell="A14" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1255,10 +1253,10 @@
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B14" s="1">
-        <v>1323</v>
+        <v>2514</v>
       </c>
       <c r="C14" s="1">
         <v>1</v>
@@ -1267,7 +1265,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -1292,10 +1290,10 @@
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="B15" s="1">
-        <v>2431</v>
+        <v>1323</v>
       </c>
       <c r="C15" s="1">
         <v>1</v>
@@ -1304,7 +1302,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -1332,10 +1330,10 @@
         <v>6</v>
       </c>
       <c r="B16" s="1">
-        <v>2461</v>
+        <v>2431</v>
       </c>
       <c r="C16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" s="1">
         <v>1</v>
@@ -1369,7 +1367,7 @@
         <v>6</v>
       </c>
       <c r="B17" s="1">
-        <v>3441</v>
+        <v>2461</v>
       </c>
       <c r="C17" s="1">
         <v>0</v>
@@ -1403,19 +1401,19 @@
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="B18" s="1">
-        <v>2113</v>
+        <v>3441</v>
       </c>
       <c r="C18" s="1">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1">
         <v>1</v>
       </c>
-      <c r="D18" s="1">
-        <v>0</v>
-      </c>
       <c r="E18" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -1443,13 +1441,13 @@
         <v>51</v>
       </c>
       <c r="B19" s="1">
-        <v>2153</v>
+        <v>2113</v>
       </c>
       <c r="C19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19" s="1">
         <v>3</v>
@@ -1477,13 +1475,13 @@
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B20" s="1">
-        <v>2000</v>
+        <v>2153</v>
       </c>
       <c r="C20" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" s="1">
         <v>1</v>
@@ -1514,10 +1512,10 @@
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B21" s="1">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="C21" s="1">
         <v>1</v>
@@ -1551,16 +1549,16 @@
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B22" s="1">
-        <v>2823</v>
+        <v>3000</v>
       </c>
       <c r="C22" s="1">
         <v>1</v>
       </c>
       <c r="D22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" s="1">
         <v>3</v>
@@ -1591,16 +1589,16 @@
         <v>54</v>
       </c>
       <c r="B23" s="1">
-        <v>2311</v>
+        <v>2823</v>
       </c>
       <c r="C23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
@@ -1628,7 +1626,7 @@
         <v>54</v>
       </c>
       <c r="B24" s="1">
-        <v>2303</v>
+        <v>2311</v>
       </c>
       <c r="C24" s="1">
         <v>0</v>
@@ -1637,7 +1635,7 @@
         <v>1</v>
       </c>
       <c r="E24" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
@@ -1665,10 +1663,10 @@
         <v>54</v>
       </c>
       <c r="B25" s="1">
-        <v>3293</v>
+        <v>2303</v>
       </c>
       <c r="C25" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D25" s="1">
         <v>1</v>
@@ -1702,16 +1700,16 @@
         <v>54</v>
       </c>
       <c r="B26" s="1">
-        <v>3304</v>
+        <v>3293</v>
       </c>
       <c r="C26" s="1">
         <v>1</v>
       </c>
       <c r="D26" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
@@ -1739,7 +1737,7 @@
         <v>54</v>
       </c>
       <c r="B27" s="1">
-        <v>4113</v>
+        <v>3304</v>
       </c>
       <c r="C27" s="1">
         <v>1</v>
@@ -1748,7 +1746,7 @@
         <v>0</v>
       </c>
       <c r="E27" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
@@ -1776,7 +1774,7 @@
         <v>54</v>
       </c>
       <c r="B28" s="1">
-        <v>4553</v>
+        <v>4113</v>
       </c>
       <c r="C28" s="1">
         <v>1</v>
@@ -1813,7 +1811,7 @@
         <v>54</v>
       </c>
       <c r="B29" s="1">
-        <v>4623</v>
+        <v>4553</v>
       </c>
       <c r="C29" s="1">
         <v>1</v>
@@ -1850,13 +1848,13 @@
         <v>54</v>
       </c>
       <c r="B30" s="1">
-        <v>4223</v>
+        <v>4623</v>
       </c>
       <c r="C30" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D30" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E30" s="1">
         <v>3</v>
@@ -1887,7 +1885,7 @@
         <v>54</v>
       </c>
       <c r="B31" s="1">
-        <v>4563</v>
+        <v>4223</v>
       </c>
       <c r="C31" s="1">
         <v>0</v>
@@ -1924,7 +1922,7 @@
         <v>54</v>
       </c>
       <c r="B32" s="1">
-        <v>4633</v>
+        <v>4563</v>
       </c>
       <c r="C32" s="1">
         <v>0</v>
@@ -1961,7 +1959,7 @@
         <v>54</v>
       </c>
       <c r="B33" s="1">
-        <v>4804</v>
+        <v>4633</v>
       </c>
       <c r="C33" s="1">
         <v>0</v>
@@ -1970,7 +1968,7 @@
         <v>1</v>
       </c>
       <c r="E33" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
@@ -1994,21 +1992,6 @@
       <c r="Y33" s="1"/>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A34" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B34" s="1">
-        <v>4333</v>
-      </c>
-      <c r="C34" s="1">
-        <v>1</v>
-      </c>
-      <c r="D34" s="1">
-        <v>0</v>
-      </c>
-      <c r="E34" s="1">
-        <v>3</v>
-      </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
@@ -2035,16 +2018,16 @@
         <v>54</v>
       </c>
       <c r="B35" s="1">
-        <v>4383</v>
+        <v>4804</v>
       </c>
       <c r="C35" s="1">
+        <v>0</v>
+      </c>
+      <c r="D35" s="1">
         <v>1</v>
       </c>
-      <c r="D35" s="1">
-        <v>0</v>
-      </c>
       <c r="E35" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
@@ -2072,7 +2055,7 @@
         <v>54</v>
       </c>
       <c r="B36" s="1">
-        <v>4663</v>
+        <v>4333</v>
       </c>
       <c r="C36" s="1">
         <v>1</v>
@@ -2109,7 +2092,7 @@
         <v>54</v>
       </c>
       <c r="B37" s="1">
-        <v>4853</v>
+        <v>4383</v>
       </c>
       <c r="C37" s="1">
         <v>1</v>
@@ -2146,13 +2129,13 @@
         <v>54</v>
       </c>
       <c r="B38" s="1">
-        <v>4393</v>
+        <v>4663</v>
       </c>
       <c r="C38" s="1">
         <v>1</v>
       </c>
       <c r="D38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E38" s="1">
         <v>3</v>
@@ -2180,19 +2163,19 @@
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B39" s="1">
-        <v>2514</v>
+        <v>4853</v>
       </c>
       <c r="C39" s="1">
         <v>1</v>
       </c>
       <c r="D39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E39" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
@@ -2216,11 +2199,21 @@
       <c r="Y39" s="1"/>
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
+      <c r="A40" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B40" s="1">
+        <v>4393</v>
+      </c>
+      <c r="C40" s="1">
+        <v>1</v>
+      </c>
+      <c r="D40" s="1">
+        <v>1</v>
+      </c>
+      <c r="E40" s="1">
+        <v>3</v>
+      </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
@@ -2243,11 +2236,6 @@
       <c r="Y40" s="1"/>
     </row>
     <row r="41" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
@@ -28277,10 +28265,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8499CC35-5328-4E88-B8A4-3963CC5E7F80}">
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -28668,7 +28656,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="B14" s="3">
         <v>1</v>
@@ -28697,7 +28685,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" s="3">
         <v>1</v>
@@ -28726,28 +28714,28 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" s="3">
         <v>1</v>
       </c>
       <c r="D16" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" s="3">
         <v>1</v>
       </c>
       <c r="F16" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" s="3">
         <v>1</v>
       </c>
       <c r="H16" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I16" s="3">
         <v>1</v>
@@ -28755,7 +28743,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" s="3">
         <v>0</v>
@@ -28784,86 +28772,86 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" s="3">
+        <v>0</v>
+      </c>
+      <c r="C18" s="3">
         <v>1</v>
       </c>
-      <c r="C18" s="3">
-        <v>0</v>
-      </c>
       <c r="D18" s="3">
+        <v>0</v>
+      </c>
+      <c r="E18" s="3">
         <v>1</v>
       </c>
-      <c r="E18" s="3">
-        <v>0</v>
-      </c>
       <c r="F18" s="3">
+        <v>0</v>
+      </c>
+      <c r="G18" s="3">
         <v>1</v>
       </c>
-      <c r="G18" s="3">
-        <v>0</v>
-      </c>
       <c r="H18" s="3">
+        <v>0</v>
+      </c>
+      <c r="I18" s="3">
         <v>1</v>
-      </c>
-      <c r="I18" s="3">
-        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19" s="3">
+        <v>0</v>
+      </c>
+      <c r="D19" s="3">
         <v>1</v>
       </c>
-      <c r="D19" s="3">
-        <v>0</v>
-      </c>
       <c r="E19" s="3">
+        <v>0</v>
+      </c>
+      <c r="F19" s="3">
         <v>1</v>
       </c>
-      <c r="F19" s="3">
-        <v>0</v>
-      </c>
       <c r="G19" s="3">
+        <v>0</v>
+      </c>
+      <c r="H19" s="3">
         <v>1</v>
       </c>
-      <c r="H19" s="3">
-        <v>0</v>
-      </c>
       <c r="I19" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B20" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20" s="3">
         <v>1</v>
       </c>
       <c r="D20" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20" s="3">
         <v>1</v>
       </c>
       <c r="F20" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G20" s="3">
         <v>1</v>
       </c>
       <c r="H20" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I20" s="3">
         <v>1</v>
@@ -28871,7 +28859,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B21" s="3">
         <v>1</v>
@@ -28900,65 +28888,65 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22" s="3">
         <v>1</v>
       </c>
       <c r="C22" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" s="3">
         <v>1</v>
       </c>
       <c r="E22" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22" s="3">
         <v>1</v>
       </c>
       <c r="G22" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22" s="3">
         <v>1</v>
       </c>
       <c r="I22" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23" s="3">
+        <v>0</v>
+      </c>
+      <c r="D23" s="3">
         <v>1</v>
       </c>
-      <c r="D23" s="3">
-        <v>0</v>
-      </c>
       <c r="E23" s="3">
+        <v>0</v>
+      </c>
+      <c r="F23" s="3">
         <v>1</v>
       </c>
-      <c r="F23" s="3">
-        <v>0</v>
-      </c>
       <c r="G23" s="3">
+        <v>0</v>
+      </c>
+      <c r="H23" s="3">
         <v>1</v>
       </c>
-      <c r="H23" s="3">
-        <v>0</v>
-      </c>
       <c r="I23" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B24" s="3">
         <v>0</v>
@@ -28987,28 +28975,28 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B25" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C25" s="3">
         <v>1</v>
       </c>
       <c r="D25" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25" s="3">
         <v>1</v>
       </c>
       <c r="F25" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G25" s="3">
         <v>1</v>
       </c>
       <c r="H25" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I25" s="3">
         <v>1</v>
@@ -29016,36 +29004,36 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B26" s="3">
         <v>1</v>
       </c>
       <c r="C26" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26" s="3">
         <v>1</v>
       </c>
       <c r="E26" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26" s="3">
         <v>1</v>
       </c>
       <c r="G26" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26" s="3">
         <v>1</v>
       </c>
       <c r="I26" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B27" s="3">
         <v>1</v>
@@ -29074,7 +29062,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B28" s="3">
         <v>1</v>
@@ -29103,7 +29091,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B29" s="3">
         <v>1</v>
@@ -29132,36 +29120,36 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B30" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C30" s="3">
+        <v>0</v>
+      </c>
+      <c r="D30" s="3">
         <v>1</v>
       </c>
-      <c r="D30" s="3">
-        <v>0</v>
-      </c>
       <c r="E30" s="3">
+        <v>0</v>
+      </c>
+      <c r="F30" s="3">
         <v>1</v>
       </c>
-      <c r="F30" s="3">
-        <v>0</v>
-      </c>
       <c r="G30" s="3">
+        <v>0</v>
+      </c>
+      <c r="H30" s="3">
         <v>1</v>
       </c>
-      <c r="H30" s="3">
-        <v>0</v>
-      </c>
       <c r="I30" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B31" s="3">
         <v>0</v>
@@ -29190,7 +29178,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B32" s="3">
         <v>0</v>
@@ -29219,7 +29207,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B33" s="3">
         <v>0</v>
@@ -29246,67 +29234,38 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A34" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B34" s="3">
-        <v>1</v>
-      </c>
-      <c r="C34" s="3">
-        <v>0</v>
-      </c>
-      <c r="D34" s="3">
-        <v>1</v>
-      </c>
-      <c r="E34" s="3">
-        <v>0</v>
-      </c>
-      <c r="F34" s="3">
-        <v>1</v>
-      </c>
-      <c r="G34" s="3">
-        <v>0</v>
-      </c>
-      <c r="H34" s="3">
-        <v>1</v>
-      </c>
-      <c r="I34" s="3">
-        <v>0</v>
-      </c>
-    </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B35" s="3">
+        <v>0</v>
+      </c>
+      <c r="C35" s="3">
         <v>1</v>
       </c>
-      <c r="C35" s="3">
-        <v>0</v>
-      </c>
       <c r="D35" s="3">
+        <v>0</v>
+      </c>
+      <c r="E35" s="3">
         <v>1</v>
       </c>
-      <c r="E35" s="3">
-        <v>0</v>
-      </c>
       <c r="F35" s="3">
+        <v>0</v>
+      </c>
+      <c r="G35" s="3">
         <v>1</v>
       </c>
-      <c r="G35" s="3">
-        <v>0</v>
-      </c>
       <c r="H35" s="3">
+        <v>0</v>
+      </c>
+      <c r="I35" s="3">
         <v>1</v>
-      </c>
-      <c r="I35" s="3">
-        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B36" s="3">
         <v>1</v>
@@ -29335,7 +29294,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B37" s="3">
         <v>1</v>
@@ -29364,59 +29323,88 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A38" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B38" s="3">
         <v>1</v>
       </c>
       <c r="C38" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D38" s="3">
         <v>1</v>
       </c>
       <c r="E38" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F38" s="3">
         <v>1</v>
       </c>
       <c r="G38" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H38" s="3">
         <v>1</v>
       </c>
       <c r="I38" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A39" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B39" s="3">
         <v>1</v>
       </c>
       <c r="C39" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D39" s="3">
         <v>1</v>
       </c>
       <c r="E39" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F39" s="3">
         <v>1</v>
       </c>
       <c r="G39" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H39" s="3">
         <v>1</v>
       </c>
       <c r="I39" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A40" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40" s="3">
+        <v>1</v>
+      </c>
+      <c r="C40" s="3">
+        <v>1</v>
+      </c>
+      <c r="D40" s="3">
+        <v>1</v>
+      </c>
+      <c r="E40" s="3">
+        <v>1</v>
+      </c>
+      <c r="F40" s="3">
+        <v>1</v>
+      </c>
+      <c r="G40" s="3">
+        <v>1</v>
+      </c>
+      <c r="H40" s="3">
+        <v>1</v>
+      </c>
+      <c r="I40" s="3">
         <v>1</v>
       </c>
     </row>
@@ -29430,8 +29418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7CDD2E9-B0AB-4B78-AAF0-949DF9D7B865}">
   <dimension ref="A1:AN1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9:H9"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -29441,7 +29429,8 @@
     <col min="3" max="4" width="8.9296875" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.53125" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.19921875" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="9.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="9.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.06640625" style="4" customWidth="1"/>
     <col min="11" max="11" width="8.73046875" style="4" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="9.19921875" style="4" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7.06640625" style="4" bestFit="1" customWidth="1"/>
@@ -73516,6 +73505,3352 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2805CA7-F238-4F23-AF6C-90621E1D8A57}">
+  <dimension ref="A1:AG33"/>
+  <sheetViews>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="X41" sqref="X41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:33" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3">
+        <v>0</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <v>0</v>
+      </c>
+      <c r="M2" s="3">
+        <v>0</v>
+      </c>
+      <c r="N2" s="3">
+        <v>0</v>
+      </c>
+      <c r="O2" s="3">
+        <v>0</v>
+      </c>
+      <c r="P2" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>0</v>
+      </c>
+      <c r="R2" s="3">
+        <v>0</v>
+      </c>
+      <c r="S2" s="3">
+        <v>0</v>
+      </c>
+      <c r="T2" s="3">
+        <v>0</v>
+      </c>
+      <c r="U2" s="3">
+        <v>0</v>
+      </c>
+      <c r="V2" s="3">
+        <v>0</v>
+      </c>
+      <c r="W2" s="3">
+        <v>0</v>
+      </c>
+      <c r="X2" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG2" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3">
+        <v>0</v>
+      </c>
+      <c r="M3" s="3">
+        <v>0</v>
+      </c>
+      <c r="N3" s="3">
+        <v>0</v>
+      </c>
+      <c r="O3" s="3">
+        <v>0</v>
+      </c>
+      <c r="P3" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>0</v>
+      </c>
+      <c r="R3" s="3">
+        <v>0</v>
+      </c>
+      <c r="S3" s="3">
+        <v>0</v>
+      </c>
+      <c r="T3" s="3">
+        <v>0</v>
+      </c>
+      <c r="U3" s="3">
+        <v>0</v>
+      </c>
+      <c r="V3" s="3">
+        <v>0</v>
+      </c>
+      <c r="W3" s="3">
+        <v>0</v>
+      </c>
+      <c r="X3" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3">
+        <v>0</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0</v>
+      </c>
+      <c r="L4" s="3">
+        <v>0</v>
+      </c>
+      <c r="M4" s="3">
+        <v>0</v>
+      </c>
+      <c r="N4" s="3">
+        <v>0</v>
+      </c>
+      <c r="O4" s="3">
+        <v>0</v>
+      </c>
+      <c r="P4" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>0</v>
+      </c>
+      <c r="R4" s="3">
+        <v>0</v>
+      </c>
+      <c r="S4" s="3">
+        <v>0</v>
+      </c>
+      <c r="T4" s="3">
+        <v>0</v>
+      </c>
+      <c r="U4" s="3">
+        <v>0</v>
+      </c>
+      <c r="V4" s="3">
+        <v>0</v>
+      </c>
+      <c r="W4" s="3">
+        <v>0</v>
+      </c>
+      <c r="X4" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0</v>
+      </c>
+      <c r="K5" s="3">
+        <v>0</v>
+      </c>
+      <c r="L5" s="3">
+        <v>0</v>
+      </c>
+      <c r="M5" s="3">
+        <v>0</v>
+      </c>
+      <c r="N5" s="3">
+        <v>0</v>
+      </c>
+      <c r="O5" s="3">
+        <v>0</v>
+      </c>
+      <c r="P5" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>0</v>
+      </c>
+      <c r="R5" s="3">
+        <v>0</v>
+      </c>
+      <c r="S5" s="3">
+        <v>0</v>
+      </c>
+      <c r="T5" s="3">
+        <v>0</v>
+      </c>
+      <c r="U5" s="3">
+        <v>0</v>
+      </c>
+      <c r="V5" s="3">
+        <v>0</v>
+      </c>
+      <c r="W5" s="3">
+        <v>0</v>
+      </c>
+      <c r="X5" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0</v>
+      </c>
+      <c r="K6" s="3">
+        <v>0</v>
+      </c>
+      <c r="L6" s="3">
+        <v>0</v>
+      </c>
+      <c r="M6" s="3">
+        <v>0</v>
+      </c>
+      <c r="N6" s="3">
+        <v>0</v>
+      </c>
+      <c r="O6" s="3">
+        <v>0</v>
+      </c>
+      <c r="P6" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>0</v>
+      </c>
+      <c r="R6" s="3">
+        <v>0</v>
+      </c>
+      <c r="S6" s="3">
+        <v>0</v>
+      </c>
+      <c r="T6" s="3">
+        <v>0</v>
+      </c>
+      <c r="U6" s="3">
+        <v>0</v>
+      </c>
+      <c r="V6" s="3">
+        <v>0</v>
+      </c>
+      <c r="W6" s="3">
+        <v>0</v>
+      </c>
+      <c r="X6" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG6" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0</v>
+      </c>
+      <c r="L7" s="3">
+        <v>0</v>
+      </c>
+      <c r="M7" s="3">
+        <v>0</v>
+      </c>
+      <c r="N7" s="3">
+        <v>0</v>
+      </c>
+      <c r="O7" s="3">
+        <v>0</v>
+      </c>
+      <c r="P7" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>0</v>
+      </c>
+      <c r="R7" s="3">
+        <v>0</v>
+      </c>
+      <c r="S7" s="3">
+        <v>0</v>
+      </c>
+      <c r="T7" s="3">
+        <v>0</v>
+      </c>
+      <c r="U7" s="3">
+        <v>0</v>
+      </c>
+      <c r="V7" s="3">
+        <v>0</v>
+      </c>
+      <c r="W7" s="3">
+        <v>0</v>
+      </c>
+      <c r="X7" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0</v>
+      </c>
+      <c r="G8" s="3">
+        <v>1</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0</v>
+      </c>
+      <c r="L8" s="3">
+        <v>0</v>
+      </c>
+      <c r="M8" s="3">
+        <v>0</v>
+      </c>
+      <c r="N8" s="3">
+        <v>0</v>
+      </c>
+      <c r="O8" s="3">
+        <v>0</v>
+      </c>
+      <c r="P8" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>0</v>
+      </c>
+      <c r="R8" s="3">
+        <v>0</v>
+      </c>
+      <c r="S8" s="3">
+        <v>0</v>
+      </c>
+      <c r="T8" s="3">
+        <v>0</v>
+      </c>
+      <c r="U8" s="3">
+        <v>0</v>
+      </c>
+      <c r="V8" s="3">
+        <v>0</v>
+      </c>
+      <c r="W8" s="3">
+        <v>0</v>
+      </c>
+      <c r="X8" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0</v>
+      </c>
+      <c r="G9" s="3">
+        <v>1</v>
+      </c>
+      <c r="H9" s="3">
+        <v>1</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0</v>
+      </c>
+      <c r="K9" s="3">
+        <v>0</v>
+      </c>
+      <c r="L9" s="3">
+        <v>0</v>
+      </c>
+      <c r="M9" s="3">
+        <v>0</v>
+      </c>
+      <c r="N9" s="3">
+        <v>0</v>
+      </c>
+      <c r="O9" s="3">
+        <v>0</v>
+      </c>
+      <c r="P9" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>0</v>
+      </c>
+      <c r="R9" s="3">
+        <v>0</v>
+      </c>
+      <c r="S9" s="3">
+        <v>0</v>
+      </c>
+      <c r="T9" s="3">
+        <v>0</v>
+      </c>
+      <c r="U9" s="3">
+        <v>0</v>
+      </c>
+      <c r="V9" s="3">
+        <v>0</v>
+      </c>
+      <c r="W9" s="3">
+        <v>0</v>
+      </c>
+      <c r="X9" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0</v>
+      </c>
+      <c r="G10" s="3">
+        <v>1</v>
+      </c>
+      <c r="H10" s="3">
+        <v>1</v>
+      </c>
+      <c r="I10" s="3">
+        <v>1</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0</v>
+      </c>
+      <c r="K10" s="3">
+        <v>0</v>
+      </c>
+      <c r="L10" s="3">
+        <v>0</v>
+      </c>
+      <c r="M10" s="3">
+        <v>0</v>
+      </c>
+      <c r="N10" s="3">
+        <v>0</v>
+      </c>
+      <c r="O10" s="3">
+        <v>0</v>
+      </c>
+      <c r="P10" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>0</v>
+      </c>
+      <c r="R10" s="3">
+        <v>0</v>
+      </c>
+      <c r="S10" s="3">
+        <v>0</v>
+      </c>
+      <c r="T10" s="3">
+        <v>0</v>
+      </c>
+      <c r="U10" s="3">
+        <v>0</v>
+      </c>
+      <c r="V10" s="3">
+        <v>0</v>
+      </c>
+      <c r="W10" s="3">
+        <v>0</v>
+      </c>
+      <c r="X10" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE10" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF10" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG10" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0</v>
+      </c>
+      <c r="G11" s="3">
+        <v>1</v>
+      </c>
+      <c r="H11" s="4">
+        <v>1</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0</v>
+      </c>
+      <c r="J11" s="3">
+        <v>0</v>
+      </c>
+      <c r="K11" s="3">
+        <v>0</v>
+      </c>
+      <c r="L11" s="3">
+        <v>0</v>
+      </c>
+      <c r="M11" s="3">
+        <v>0</v>
+      </c>
+      <c r="N11" s="3">
+        <v>1</v>
+      </c>
+      <c r="O11" s="3">
+        <v>0</v>
+      </c>
+      <c r="P11" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>0</v>
+      </c>
+      <c r="R11" s="3">
+        <v>0</v>
+      </c>
+      <c r="S11" s="3">
+        <v>0</v>
+      </c>
+      <c r="T11" s="3">
+        <v>0</v>
+      </c>
+      <c r="U11" s="3">
+        <v>0</v>
+      </c>
+      <c r="V11" s="3">
+        <v>0</v>
+      </c>
+      <c r="W11" s="3">
+        <v>0</v>
+      </c>
+      <c r="X11" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0</v>
+      </c>
+      <c r="J12" s="3">
+        <v>0</v>
+      </c>
+      <c r="K12" s="3">
+        <v>0</v>
+      </c>
+      <c r="L12" s="3">
+        <v>0</v>
+      </c>
+      <c r="M12" s="3">
+        <v>0</v>
+      </c>
+      <c r="N12" s="3">
+        <v>0</v>
+      </c>
+      <c r="O12" s="3">
+        <v>0</v>
+      </c>
+      <c r="P12" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>0</v>
+      </c>
+      <c r="R12" s="3">
+        <v>0</v>
+      </c>
+      <c r="S12" s="3">
+        <v>0</v>
+      </c>
+      <c r="T12" s="3">
+        <v>0</v>
+      </c>
+      <c r="U12" s="3">
+        <v>0</v>
+      </c>
+      <c r="V12" s="3">
+        <v>0</v>
+      </c>
+      <c r="W12" s="3">
+        <v>0</v>
+      </c>
+      <c r="X12" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD12" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE12" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF12" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0</v>
+      </c>
+      <c r="H13" s="3">
+        <v>0</v>
+      </c>
+      <c r="I13" s="3">
+        <v>0</v>
+      </c>
+      <c r="J13" s="3">
+        <v>0</v>
+      </c>
+      <c r="K13" s="3">
+        <v>0</v>
+      </c>
+      <c r="L13" s="3">
+        <v>0</v>
+      </c>
+      <c r="M13" s="3">
+        <v>0</v>
+      </c>
+      <c r="N13" s="3">
+        <v>0</v>
+      </c>
+      <c r="O13" s="3">
+        <v>0</v>
+      </c>
+      <c r="P13" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>0</v>
+      </c>
+      <c r="R13" s="3">
+        <v>0</v>
+      </c>
+      <c r="S13" s="3">
+        <v>0</v>
+      </c>
+      <c r="T13" s="3">
+        <v>0</v>
+      </c>
+      <c r="U13" s="3">
+        <v>0</v>
+      </c>
+      <c r="V13" s="3">
+        <v>0</v>
+      </c>
+      <c r="W13" s="3">
+        <v>0</v>
+      </c>
+      <c r="X13" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD13" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE13" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF13" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG13" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A14" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="3">
+        <v>0</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0</v>
+      </c>
+      <c r="G14" s="3">
+        <v>1</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0</v>
+      </c>
+      <c r="I14" s="3">
+        <v>0</v>
+      </c>
+      <c r="J14" s="3">
+        <v>0</v>
+      </c>
+      <c r="K14" s="3">
+        <v>0</v>
+      </c>
+      <c r="L14" s="3">
+        <v>0</v>
+      </c>
+      <c r="M14" s="3">
+        <v>0</v>
+      </c>
+      <c r="N14" s="3">
+        <v>0</v>
+      </c>
+      <c r="O14" s="3">
+        <v>0</v>
+      </c>
+      <c r="P14" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>0</v>
+      </c>
+      <c r="R14" s="3">
+        <v>0</v>
+      </c>
+      <c r="S14" s="3">
+        <v>0</v>
+      </c>
+      <c r="T14" s="3">
+        <v>0</v>
+      </c>
+      <c r="U14" s="3">
+        <v>0</v>
+      </c>
+      <c r="V14" s="3">
+        <v>0</v>
+      </c>
+      <c r="W14" s="3">
+        <v>0</v>
+      </c>
+      <c r="X14" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD14" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE14" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF14" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG14" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A15" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="3">
+        <v>0</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0</v>
+      </c>
+      <c r="H15" s="3">
+        <v>0</v>
+      </c>
+      <c r="I15" s="3">
+        <v>0</v>
+      </c>
+      <c r="J15" s="3">
+        <v>0</v>
+      </c>
+      <c r="K15" s="3">
+        <v>0</v>
+      </c>
+      <c r="L15" s="3">
+        <v>0</v>
+      </c>
+      <c r="M15" s="3">
+        <v>0</v>
+      </c>
+      <c r="N15" s="3">
+        <v>0</v>
+      </c>
+      <c r="O15" s="3">
+        <v>0</v>
+      </c>
+      <c r="P15" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>0</v>
+      </c>
+      <c r="R15" s="3">
+        <v>0</v>
+      </c>
+      <c r="S15" s="3">
+        <v>0</v>
+      </c>
+      <c r="T15" s="3">
+        <v>0</v>
+      </c>
+      <c r="U15" s="3">
+        <v>0</v>
+      </c>
+      <c r="V15" s="3">
+        <v>0</v>
+      </c>
+      <c r="W15" s="3">
+        <v>0</v>
+      </c>
+      <c r="X15" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB15" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC15" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD15" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE15" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF15" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG15" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0</v>
+      </c>
+      <c r="G16" s="3">
+        <v>1</v>
+      </c>
+      <c r="H16" s="3">
+        <v>1</v>
+      </c>
+      <c r="I16" s="3">
+        <v>0</v>
+      </c>
+      <c r="J16" s="3">
+        <v>0</v>
+      </c>
+      <c r="K16" s="3">
+        <v>1</v>
+      </c>
+      <c r="L16" s="3">
+        <v>0</v>
+      </c>
+      <c r="M16" s="3">
+        <v>0</v>
+      </c>
+      <c r="N16" s="3">
+        <v>1</v>
+      </c>
+      <c r="O16" s="3">
+        <v>0</v>
+      </c>
+      <c r="P16" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>0</v>
+      </c>
+      <c r="R16" s="3">
+        <v>0</v>
+      </c>
+      <c r="S16" s="3">
+        <v>0</v>
+      </c>
+      <c r="T16" s="3">
+        <v>0</v>
+      </c>
+      <c r="U16" s="3">
+        <v>0</v>
+      </c>
+      <c r="V16" s="3">
+        <v>0</v>
+      </c>
+      <c r="W16" s="3">
+        <v>0</v>
+      </c>
+      <c r="X16" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC16" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD16" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE16" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF16" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:33" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A17" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="3">
+        <v>0</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0</v>
+      </c>
+      <c r="G17" s="3">
+        <v>1</v>
+      </c>
+      <c r="H17" s="3">
+        <v>1</v>
+      </c>
+      <c r="I17" s="3">
+        <v>0</v>
+      </c>
+      <c r="J17" s="3">
+        <v>0</v>
+      </c>
+      <c r="K17" s="3">
+        <v>1</v>
+      </c>
+      <c r="L17" s="3">
+        <v>0</v>
+      </c>
+      <c r="M17" s="3">
+        <v>0</v>
+      </c>
+      <c r="N17" s="3">
+        <v>1</v>
+      </c>
+      <c r="O17" s="3">
+        <v>0</v>
+      </c>
+      <c r="P17" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>0</v>
+      </c>
+      <c r="R17" s="3">
+        <v>0</v>
+      </c>
+      <c r="S17" s="3">
+        <v>0</v>
+      </c>
+      <c r="T17" s="3">
+        <v>0</v>
+      </c>
+      <c r="U17" s="3">
+        <v>0</v>
+      </c>
+      <c r="V17" s="3">
+        <v>0</v>
+      </c>
+      <c r="W17" s="3">
+        <v>0</v>
+      </c>
+      <c r="X17" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC17" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD17" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE17" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF17" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG17" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:33" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A18" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="3">
+        <v>0</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0</v>
+      </c>
+      <c r="G18" s="3">
+        <v>0</v>
+      </c>
+      <c r="H18" s="3">
+        <v>0</v>
+      </c>
+      <c r="I18" s="3">
+        <v>0</v>
+      </c>
+      <c r="J18" s="3">
+        <v>0</v>
+      </c>
+      <c r="K18" s="3">
+        <v>0</v>
+      </c>
+      <c r="L18" s="3">
+        <v>0</v>
+      </c>
+      <c r="M18" s="3">
+        <v>0</v>
+      </c>
+      <c r="N18" s="3">
+        <v>0</v>
+      </c>
+      <c r="O18" s="3">
+        <v>0</v>
+      </c>
+      <c r="P18" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>0</v>
+      </c>
+      <c r="R18" s="3">
+        <v>0</v>
+      </c>
+      <c r="S18" s="3">
+        <v>0</v>
+      </c>
+      <c r="T18" s="3">
+        <v>0</v>
+      </c>
+      <c r="U18" s="3">
+        <v>0</v>
+      </c>
+      <c r="V18" s="3">
+        <v>0</v>
+      </c>
+      <c r="W18" s="3">
+        <v>0</v>
+      </c>
+      <c r="X18" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD18" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE18" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF18" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG18" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A19" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="3">
+        <v>0</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0</v>
+      </c>
+      <c r="G19" s="3">
+        <v>1</v>
+      </c>
+      <c r="H19" s="3">
+        <v>0</v>
+      </c>
+      <c r="I19" s="3">
+        <v>0</v>
+      </c>
+      <c r="J19" s="3">
+        <v>0</v>
+      </c>
+      <c r="K19" s="3">
+        <v>0</v>
+      </c>
+      <c r="L19" s="3">
+        <v>0</v>
+      </c>
+      <c r="M19" s="3">
+        <v>0</v>
+      </c>
+      <c r="N19" s="3">
+        <v>1</v>
+      </c>
+      <c r="O19" s="3">
+        <v>0</v>
+      </c>
+      <c r="P19" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="3">
+        <v>0</v>
+      </c>
+      <c r="R19" s="3">
+        <v>0</v>
+      </c>
+      <c r="S19" s="3">
+        <v>0</v>
+      </c>
+      <c r="T19" s="3">
+        <v>0</v>
+      </c>
+      <c r="U19" s="3">
+        <v>0</v>
+      </c>
+      <c r="V19" s="3">
+        <v>0</v>
+      </c>
+      <c r="W19" s="3">
+        <v>0</v>
+      </c>
+      <c r="X19" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG19" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A20" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="3">
+        <v>0</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0</v>
+      </c>
+      <c r="G20" s="3">
+        <v>1</v>
+      </c>
+      <c r="H20" s="3">
+        <v>0</v>
+      </c>
+      <c r="I20" s="3">
+        <v>0</v>
+      </c>
+      <c r="J20" s="3">
+        <v>0</v>
+      </c>
+      <c r="K20" s="3">
+        <v>0</v>
+      </c>
+      <c r="L20" s="3">
+        <v>0</v>
+      </c>
+      <c r="M20" s="3">
+        <v>0</v>
+      </c>
+      <c r="N20" s="3">
+        <v>1</v>
+      </c>
+      <c r="O20" s="3">
+        <v>0</v>
+      </c>
+      <c r="P20" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="3">
+        <v>0</v>
+      </c>
+      <c r="R20" s="3">
+        <v>0</v>
+      </c>
+      <c r="S20" s="3">
+        <v>1</v>
+      </c>
+      <c r="T20" s="3">
+        <v>0</v>
+      </c>
+      <c r="U20" s="3">
+        <v>0</v>
+      </c>
+      <c r="V20" s="3">
+        <v>0</v>
+      </c>
+      <c r="W20" s="3">
+        <v>0</v>
+      </c>
+      <c r="X20" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG20" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A21" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="3">
+        <v>0</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0</v>
+      </c>
+      <c r="F21" s="3">
+        <v>0</v>
+      </c>
+      <c r="G21" s="3">
+        <v>0</v>
+      </c>
+      <c r="H21" s="3">
+        <v>0</v>
+      </c>
+      <c r="I21" s="3">
+        <v>0</v>
+      </c>
+      <c r="J21" s="3">
+        <v>0</v>
+      </c>
+      <c r="K21" s="3">
+        <v>0</v>
+      </c>
+      <c r="L21" s="3">
+        <v>0</v>
+      </c>
+      <c r="M21" s="3">
+        <v>0</v>
+      </c>
+      <c r="N21" s="3">
+        <v>0</v>
+      </c>
+      <c r="O21" s="3">
+        <v>0</v>
+      </c>
+      <c r="P21" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>0</v>
+      </c>
+      <c r="R21" s="3">
+        <v>0</v>
+      </c>
+      <c r="S21" s="3">
+        <v>0</v>
+      </c>
+      <c r="T21" s="3">
+        <v>0</v>
+      </c>
+      <c r="U21" s="3">
+        <v>0</v>
+      </c>
+      <c r="V21" s="3">
+        <v>0</v>
+      </c>
+      <c r="W21" s="3">
+        <v>0</v>
+      </c>
+      <c r="X21" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y21" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG21" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A22" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="3">
+        <v>0</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0</v>
+      </c>
+      <c r="F22" s="3">
+        <v>0</v>
+      </c>
+      <c r="G22" s="3">
+        <v>0</v>
+      </c>
+      <c r="H22" s="3">
+        <v>0</v>
+      </c>
+      <c r="I22" s="3">
+        <v>0</v>
+      </c>
+      <c r="J22" s="3">
+        <v>0</v>
+      </c>
+      <c r="K22" s="3">
+        <v>0</v>
+      </c>
+      <c r="L22" s="3">
+        <v>0</v>
+      </c>
+      <c r="M22" s="3">
+        <v>0</v>
+      </c>
+      <c r="N22" s="3">
+        <v>0</v>
+      </c>
+      <c r="O22" s="3">
+        <v>0</v>
+      </c>
+      <c r="P22" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>0</v>
+      </c>
+      <c r="R22" s="3">
+        <v>0</v>
+      </c>
+      <c r="S22" s="3">
+        <v>0</v>
+      </c>
+      <c r="T22" s="3">
+        <v>0</v>
+      </c>
+      <c r="U22" s="3">
+        <v>0</v>
+      </c>
+      <c r="V22" s="3">
+        <v>0</v>
+      </c>
+      <c r="W22" s="3">
+        <v>0</v>
+      </c>
+      <c r="X22" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG22" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A23" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="3">
+        <v>0</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0</v>
+      </c>
+      <c r="F23" s="3">
+        <v>0</v>
+      </c>
+      <c r="G23" s="3">
+        <v>0</v>
+      </c>
+      <c r="H23" s="3">
+        <v>0</v>
+      </c>
+      <c r="I23" s="3">
+        <v>0</v>
+      </c>
+      <c r="J23" s="3">
+        <v>0</v>
+      </c>
+      <c r="K23" s="3">
+        <v>0</v>
+      </c>
+      <c r="L23" s="3">
+        <v>0</v>
+      </c>
+      <c r="M23" s="3">
+        <v>0</v>
+      </c>
+      <c r="N23" s="3">
+        <v>0</v>
+      </c>
+      <c r="O23" s="3">
+        <v>0</v>
+      </c>
+      <c r="P23" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="3">
+        <v>0</v>
+      </c>
+      <c r="R23" s="3">
+        <v>0</v>
+      </c>
+      <c r="S23" s="3">
+        <v>0</v>
+      </c>
+      <c r="T23" s="3">
+        <v>0</v>
+      </c>
+      <c r="U23" s="3">
+        <v>0</v>
+      </c>
+      <c r="V23" s="3">
+        <v>0</v>
+      </c>
+      <c r="W23" s="3">
+        <v>0</v>
+      </c>
+      <c r="X23" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y23" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG23" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A24" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="3">
+        <v>0</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0</v>
+      </c>
+      <c r="E24" s="3">
+        <v>0</v>
+      </c>
+      <c r="F24" s="3">
+        <v>0</v>
+      </c>
+      <c r="G24" s="3">
+        <v>0</v>
+      </c>
+      <c r="H24" s="3">
+        <v>0</v>
+      </c>
+      <c r="I24" s="3">
+        <v>0</v>
+      </c>
+      <c r="J24" s="3">
+        <v>0</v>
+      </c>
+      <c r="K24" s="3">
+        <v>0</v>
+      </c>
+      <c r="L24" s="3">
+        <v>0</v>
+      </c>
+      <c r="M24" s="3">
+        <v>0</v>
+      </c>
+      <c r="N24" s="3">
+        <v>0</v>
+      </c>
+      <c r="O24" s="3">
+        <v>0</v>
+      </c>
+      <c r="P24" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="3">
+        <v>0</v>
+      </c>
+      <c r="R24" s="3">
+        <v>0</v>
+      </c>
+      <c r="S24" s="3">
+        <v>0</v>
+      </c>
+      <c r="T24" s="3">
+        <v>0</v>
+      </c>
+      <c r="U24" s="3">
+        <v>0</v>
+      </c>
+      <c r="V24" s="3">
+        <v>0</v>
+      </c>
+      <c r="W24" s="3">
+        <v>0</v>
+      </c>
+      <c r="X24" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y24" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z24" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA24" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB24" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC24" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD24" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE24" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF24" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG24" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A25" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="3">
+        <v>0</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0</v>
+      </c>
+      <c r="E25" s="3">
+        <v>0</v>
+      </c>
+      <c r="F25" s="3">
+        <v>0</v>
+      </c>
+      <c r="G25" s="3">
+        <v>1</v>
+      </c>
+      <c r="H25" s="3">
+        <v>0</v>
+      </c>
+      <c r="I25" s="3">
+        <v>0</v>
+      </c>
+      <c r="J25" s="3">
+        <v>0</v>
+      </c>
+      <c r="K25" s="3">
+        <v>0</v>
+      </c>
+      <c r="L25" s="3">
+        <v>0</v>
+      </c>
+      <c r="M25" s="3">
+        <v>0</v>
+      </c>
+      <c r="N25" s="3">
+        <v>1</v>
+      </c>
+      <c r="O25" s="3">
+        <v>0</v>
+      </c>
+      <c r="P25" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="3">
+        <v>0</v>
+      </c>
+      <c r="R25" s="3">
+        <v>0</v>
+      </c>
+      <c r="S25" s="3">
+        <v>1</v>
+      </c>
+      <c r="T25" s="3">
+        <v>0</v>
+      </c>
+      <c r="U25" s="3">
+        <v>0</v>
+      </c>
+      <c r="V25" s="3">
+        <v>0</v>
+      </c>
+      <c r="W25" s="3">
+        <v>0</v>
+      </c>
+      <c r="X25" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y25" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z25" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA25" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB25" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC25" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD25" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE25" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF25" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG25" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A26" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="3">
+        <v>0</v>
+      </c>
+      <c r="C26" s="3">
+        <v>0</v>
+      </c>
+      <c r="D26" s="3">
+        <v>0</v>
+      </c>
+      <c r="E26" s="3">
+        <v>0</v>
+      </c>
+      <c r="F26" s="3">
+        <v>0</v>
+      </c>
+      <c r="G26" s="3">
+        <v>0</v>
+      </c>
+      <c r="H26" s="3">
+        <v>0</v>
+      </c>
+      <c r="I26" s="3">
+        <v>0</v>
+      </c>
+      <c r="J26" s="3">
+        <v>0</v>
+      </c>
+      <c r="K26" s="3">
+        <v>0</v>
+      </c>
+      <c r="L26" s="3">
+        <v>0</v>
+      </c>
+      <c r="M26" s="3">
+        <v>0</v>
+      </c>
+      <c r="N26" s="3">
+        <v>0</v>
+      </c>
+      <c r="O26" s="3">
+        <v>0</v>
+      </c>
+      <c r="P26" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="3">
+        <v>0</v>
+      </c>
+      <c r="R26" s="3">
+        <v>0</v>
+      </c>
+      <c r="S26" s="3">
+        <v>0</v>
+      </c>
+      <c r="T26" s="3">
+        <v>0</v>
+      </c>
+      <c r="U26" s="3">
+        <v>0</v>
+      </c>
+      <c r="V26" s="3">
+        <v>0</v>
+      </c>
+      <c r="W26" s="3">
+        <v>0</v>
+      </c>
+      <c r="X26" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y26" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z26" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA26" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB26" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC26" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD26" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE26" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF26" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG26" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A27" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="3">
+        <v>0</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0</v>
+      </c>
+      <c r="D27" s="3">
+        <v>0</v>
+      </c>
+      <c r="E27" s="3">
+        <v>0</v>
+      </c>
+      <c r="F27" s="3">
+        <v>0</v>
+      </c>
+      <c r="G27" s="3">
+        <v>1</v>
+      </c>
+      <c r="H27" s="3">
+        <v>0</v>
+      </c>
+      <c r="I27" s="3">
+        <v>0</v>
+      </c>
+      <c r="J27" s="3">
+        <v>0</v>
+      </c>
+      <c r="K27" s="3">
+        <v>0</v>
+      </c>
+      <c r="L27" s="3">
+        <v>0</v>
+      </c>
+      <c r="M27" s="3">
+        <v>0</v>
+      </c>
+      <c r="N27" s="3">
+        <v>1</v>
+      </c>
+      <c r="O27" s="3">
+        <v>0</v>
+      </c>
+      <c r="P27" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="3">
+        <v>0</v>
+      </c>
+      <c r="R27" s="3">
+        <v>0</v>
+      </c>
+      <c r="S27" s="3">
+        <v>1</v>
+      </c>
+      <c r="T27" s="3">
+        <v>1</v>
+      </c>
+      <c r="U27" s="3">
+        <v>0</v>
+      </c>
+      <c r="V27" s="3">
+        <v>0</v>
+      </c>
+      <c r="W27" s="3">
+        <v>0</v>
+      </c>
+      <c r="X27" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y27" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z27" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA27" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB27" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC27" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD27" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE27" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF27" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG27" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A28" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="3">
+        <v>0</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0</v>
+      </c>
+      <c r="D28" s="3">
+        <v>0</v>
+      </c>
+      <c r="E28" s="3">
+        <v>0</v>
+      </c>
+      <c r="F28" s="3">
+        <v>0</v>
+      </c>
+      <c r="G28" s="3">
+        <v>0</v>
+      </c>
+      <c r="H28" s="3">
+        <v>0</v>
+      </c>
+      <c r="I28" s="3">
+        <v>0</v>
+      </c>
+      <c r="J28" s="3">
+        <v>0</v>
+      </c>
+      <c r="K28" s="3">
+        <v>0</v>
+      </c>
+      <c r="L28" s="3">
+        <v>0</v>
+      </c>
+      <c r="M28" s="3">
+        <v>0</v>
+      </c>
+      <c r="N28" s="3">
+        <v>0</v>
+      </c>
+      <c r="O28" s="3">
+        <v>1</v>
+      </c>
+      <c r="P28" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="3">
+        <v>0</v>
+      </c>
+      <c r="R28" s="3">
+        <v>0</v>
+      </c>
+      <c r="S28" s="3">
+        <v>0</v>
+      </c>
+      <c r="T28" s="3">
+        <v>0</v>
+      </c>
+      <c r="U28" s="3">
+        <v>0</v>
+      </c>
+      <c r="V28" s="3">
+        <v>0</v>
+      </c>
+      <c r="W28" s="3">
+        <v>0</v>
+      </c>
+      <c r="X28" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y28" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z28" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA28" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB28" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC28" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD28" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE28" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF28" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG28" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A29" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="3">
+        <v>0</v>
+      </c>
+      <c r="C29" s="3">
+        <v>0</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0</v>
+      </c>
+      <c r="E29" s="3">
+        <v>0</v>
+      </c>
+      <c r="F29" s="3">
+        <v>0</v>
+      </c>
+      <c r="G29" s="3">
+        <v>0</v>
+      </c>
+      <c r="H29" s="3">
+        <v>0</v>
+      </c>
+      <c r="I29" s="3">
+        <v>0</v>
+      </c>
+      <c r="J29" s="3">
+        <v>0</v>
+      </c>
+      <c r="K29" s="3">
+        <v>0</v>
+      </c>
+      <c r="L29" s="3">
+        <v>0</v>
+      </c>
+      <c r="M29" s="3">
+        <v>0</v>
+      </c>
+      <c r="N29" s="3">
+        <v>0</v>
+      </c>
+      <c r="O29" s="3">
+        <v>0</v>
+      </c>
+      <c r="P29" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="3">
+        <v>0</v>
+      </c>
+      <c r="R29" s="3">
+        <v>0</v>
+      </c>
+      <c r="S29" s="3">
+        <v>0</v>
+      </c>
+      <c r="T29" s="3">
+        <v>0</v>
+      </c>
+      <c r="U29" s="3">
+        <v>0</v>
+      </c>
+      <c r="V29" s="3">
+        <v>0</v>
+      </c>
+      <c r="W29" s="3">
+        <v>0</v>
+      </c>
+      <c r="X29" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y29" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z29" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA29" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB29" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC29" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD29" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE29" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF29" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG29" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A30" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" s="3">
+        <v>0</v>
+      </c>
+      <c r="C30" s="3">
+        <v>0</v>
+      </c>
+      <c r="D30" s="3">
+        <v>0</v>
+      </c>
+      <c r="E30" s="3">
+        <v>0</v>
+      </c>
+      <c r="F30" s="3">
+        <v>0</v>
+      </c>
+      <c r="G30" s="3">
+        <v>0</v>
+      </c>
+      <c r="H30" s="3">
+        <v>0</v>
+      </c>
+      <c r="I30" s="3">
+        <v>0</v>
+      </c>
+      <c r="J30" s="3">
+        <v>0</v>
+      </c>
+      <c r="K30" s="3">
+        <v>0</v>
+      </c>
+      <c r="L30" s="3">
+        <v>0</v>
+      </c>
+      <c r="M30" s="3">
+        <v>0</v>
+      </c>
+      <c r="N30" s="3">
+        <v>0</v>
+      </c>
+      <c r="O30" s="3">
+        <v>0</v>
+      </c>
+      <c r="P30" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="3">
+        <v>0</v>
+      </c>
+      <c r="R30" s="3">
+        <v>0</v>
+      </c>
+      <c r="S30" s="3">
+        <v>0</v>
+      </c>
+      <c r="T30" s="3">
+        <v>0</v>
+      </c>
+      <c r="U30" s="3">
+        <v>0</v>
+      </c>
+      <c r="V30" s="3">
+        <v>0</v>
+      </c>
+      <c r="W30" s="3">
+        <v>1</v>
+      </c>
+      <c r="X30" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y30" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z30" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA30" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB30" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC30" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD30" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE30" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF30" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG30" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A31" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" s="3">
+        <v>0</v>
+      </c>
+      <c r="C31" s="3">
+        <v>0</v>
+      </c>
+      <c r="D31" s="3">
+        <v>0</v>
+      </c>
+      <c r="E31" s="3">
+        <v>0</v>
+      </c>
+      <c r="F31" s="3">
+        <v>0</v>
+      </c>
+      <c r="G31" s="3">
+        <v>0</v>
+      </c>
+      <c r="H31" s="3">
+        <v>0</v>
+      </c>
+      <c r="I31" s="3">
+        <v>0</v>
+      </c>
+      <c r="J31" s="3">
+        <v>0</v>
+      </c>
+      <c r="K31" s="3">
+        <v>0</v>
+      </c>
+      <c r="L31" s="3">
+        <v>0</v>
+      </c>
+      <c r="M31" s="3">
+        <v>0</v>
+      </c>
+      <c r="N31" s="3">
+        <v>0</v>
+      </c>
+      <c r="O31" s="3">
+        <v>0</v>
+      </c>
+      <c r="P31" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="3">
+        <v>0</v>
+      </c>
+      <c r="R31" s="3">
+        <v>0</v>
+      </c>
+      <c r="S31" s="3">
+        <v>0</v>
+      </c>
+      <c r="T31" s="3">
+        <v>0</v>
+      </c>
+      <c r="U31" s="3">
+        <v>0</v>
+      </c>
+      <c r="V31" s="3">
+        <v>0</v>
+      </c>
+      <c r="W31" s="3">
+        <v>0</v>
+      </c>
+      <c r="X31" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y31" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z31" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA31" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB31" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC31" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD31" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE31" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF31" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG31" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A32" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" s="3">
+        <v>0</v>
+      </c>
+      <c r="C32" s="3">
+        <v>0</v>
+      </c>
+      <c r="D32" s="3">
+        <v>0</v>
+      </c>
+      <c r="E32" s="3">
+        <v>0</v>
+      </c>
+      <c r="F32" s="3">
+        <v>0</v>
+      </c>
+      <c r="G32" s="3">
+        <v>0</v>
+      </c>
+      <c r="H32" s="3">
+        <v>0</v>
+      </c>
+      <c r="I32" s="3">
+        <v>0</v>
+      </c>
+      <c r="J32" s="3">
+        <v>0</v>
+      </c>
+      <c r="K32" s="3">
+        <v>0</v>
+      </c>
+      <c r="L32" s="3">
+        <v>0</v>
+      </c>
+      <c r="M32" s="3">
+        <v>0</v>
+      </c>
+      <c r="N32" s="3">
+        <v>0</v>
+      </c>
+      <c r="O32" s="3">
+        <v>0</v>
+      </c>
+      <c r="P32" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="3">
+        <v>0</v>
+      </c>
+      <c r="R32" s="3">
+        <v>0</v>
+      </c>
+      <c r="S32" s="3">
+        <v>0</v>
+      </c>
+      <c r="T32" s="3">
+        <v>0</v>
+      </c>
+      <c r="U32" s="3">
+        <v>0</v>
+      </c>
+      <c r="V32" s="3">
+        <v>0</v>
+      </c>
+      <c r="W32" s="3">
+        <v>0</v>
+      </c>
+      <c r="X32" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y32" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z32" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA32" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB32" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC32" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD32" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE32" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF32" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG32" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A33" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33" s="3">
+        <v>0</v>
+      </c>
+      <c r="C33" s="3">
+        <v>0</v>
+      </c>
+      <c r="D33" s="3">
+        <v>0</v>
+      </c>
+      <c r="E33" s="3">
+        <v>0</v>
+      </c>
+      <c r="F33" s="3">
+        <v>0</v>
+      </c>
+      <c r="G33" s="3">
+        <v>0</v>
+      </c>
+      <c r="H33" s="3">
+        <v>0</v>
+      </c>
+      <c r="I33" s="3">
+        <v>0</v>
+      </c>
+      <c r="J33" s="3">
+        <v>0</v>
+      </c>
+      <c r="K33" s="3">
+        <v>0</v>
+      </c>
+      <c r="L33" s="3">
+        <v>0</v>
+      </c>
+      <c r="M33" s="3">
+        <v>0</v>
+      </c>
+      <c r="N33" s="3">
+        <v>0</v>
+      </c>
+      <c r="O33" s="3">
+        <v>0</v>
+      </c>
+      <c r="P33" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="3">
+        <v>0</v>
+      </c>
+      <c r="R33" s="3">
+        <v>0</v>
+      </c>
+      <c r="S33" s="3">
+        <v>0</v>
+      </c>
+      <c r="T33" s="3">
+        <v>0</v>
+      </c>
+      <c r="U33" s="3">
+        <v>0</v>
+      </c>
+      <c r="V33" s="3">
+        <v>0</v>
+      </c>
+      <c r="W33" s="3">
+        <v>1</v>
+      </c>
+      <c r="X33" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y33" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z33" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA33" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB33" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC33" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD33" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE33" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF33" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG33" s="3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D099514-66A9-40BB-8236-071D2A75DD12}">
   <dimension ref="A1:Q97"/>
   <sheetViews>
@@ -74314,62 +77649,62 @@
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
     </row>
-    <row r="42" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="43" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="44" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="45" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="46" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="47" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="48" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="49" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="50" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="51" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="52" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="53" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="54" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="55" s="14" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="56" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="57" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="58" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="59" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="60" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="61" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="62" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="63" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="64" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="65" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="66" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="67" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="68" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="69" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="70" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="71" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="72" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="73" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="74" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="75" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="76" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="77" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="78" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="79" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="80" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="81" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="82" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="83" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="84" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="85" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="86" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="87" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="88" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="89" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="90" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="91" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="92" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="93" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="94" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="95" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="96" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="97" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="42" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="43" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="44" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="45" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="46" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="47" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="48" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="49" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="50" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="51" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="52" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="53" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="54" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="55" s="7" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="56" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="57" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="58" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="59" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="60" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="61" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="62" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="63" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="64" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="65" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="66" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="67" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="68" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="69" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="70" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="71" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="72" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="73" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="74" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="75" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="76" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="77" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="78" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="79" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="80" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="81" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="82" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="83" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="84" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="85" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="86" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="87" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="88" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="89" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="90" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="91" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="92" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="93" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="94" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="95" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="96" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="97" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Progress on the optimization
</commit_message>
<xml_diff>
--- a/Schedule-Data.xlsx
+++ b/Schedule-Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\pipe\Shaman\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5AE4B88-078E-4E83-8CA5-B7BFD3FE471A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B9F029E-5473-4F35-9A73-D78C7813ECD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" activeTab="2" xr2:uid="{503009C4-0C10-4696-AB1F-D7C487AD1E49}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" activeTab="3" xr2:uid="{503009C4-0C10-4696-AB1F-D7C487AD1E49}"/>
   </bookViews>
   <sheets>
     <sheet name="ISE" sheetId="1" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="65">
   <si>
     <t>Fall</t>
   </si>
@@ -402,7 +402,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -424,6 +424,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -461,9 +464,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -501,7 +504,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -607,7 +610,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -749,7 +752,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -759,8 +762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D6FC798-9B17-413F-A36C-134B42F149EF}">
   <dimension ref="A1:Y1004"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:E33"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1992,6 +1995,21 @@
       <c r="Y33" s="1"/>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A34" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" s="1">
+        <v>4804</v>
+      </c>
+      <c r="C34" s="1">
+        <v>0</v>
+      </c>
+      <c r="D34" s="1">
+        <v>1</v>
+      </c>
+      <c r="E34" s="1">
+        <v>4</v>
+      </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
@@ -2018,16 +2036,16 @@
         <v>54</v>
       </c>
       <c r="B35" s="1">
-        <v>4804</v>
+        <v>4333</v>
       </c>
       <c r="C35" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E35" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
@@ -2055,7 +2073,7 @@
         <v>54</v>
       </c>
       <c r="B36" s="1">
-        <v>4333</v>
+        <v>4383</v>
       </c>
       <c r="C36" s="1">
         <v>1</v>
@@ -2092,7 +2110,7 @@
         <v>54</v>
       </c>
       <c r="B37" s="1">
-        <v>4383</v>
+        <v>4663</v>
       </c>
       <c r="C37" s="1">
         <v>1</v>
@@ -2129,7 +2147,7 @@
         <v>54</v>
       </c>
       <c r="B38" s="1">
-        <v>4663</v>
+        <v>4853</v>
       </c>
       <c r="C38" s="1">
         <v>1</v>
@@ -2166,13 +2184,13 @@
         <v>54</v>
       </c>
       <c r="B39" s="1">
-        <v>4853</v>
+        <v>4393</v>
       </c>
       <c r="C39" s="1">
         <v>1</v>
       </c>
       <c r="D39" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E39" s="1">
         <v>3</v>
@@ -2199,21 +2217,6 @@
       <c r="Y39" s="1"/>
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A40" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B40" s="1">
-        <v>4393</v>
-      </c>
-      <c r="C40" s="1">
-        <v>1</v>
-      </c>
-      <c r="D40" s="1">
-        <v>1</v>
-      </c>
-      <c r="E40" s="1">
-        <v>3</v>
-      </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
@@ -28265,10 +28268,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8499CC35-5328-4E88-B8A4-3963CC5E7F80}">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+    <sheetView zoomScale="153" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -29234,38 +29237,67 @@
         <v>1</v>
       </c>
     </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A34" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" s="3">
+        <v>0</v>
+      </c>
+      <c r="C34" s="3">
+        <v>1</v>
+      </c>
+      <c r="D34" s="3">
+        <v>0</v>
+      </c>
+      <c r="E34" s="3">
+        <v>1</v>
+      </c>
+      <c r="F34" s="3">
+        <v>0</v>
+      </c>
+      <c r="G34" s="3">
+        <v>1</v>
+      </c>
+      <c r="H34" s="3">
+        <v>0</v>
+      </c>
+      <c r="I34" s="3">
+        <v>1</v>
+      </c>
+    </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B35" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C35" s="3">
+        <v>0</v>
+      </c>
+      <c r="D35" s="3">
         <v>1</v>
       </c>
-      <c r="D35" s="3">
-        <v>0</v>
-      </c>
       <c r="E35" s="3">
+        <v>0</v>
+      </c>
+      <c r="F35" s="3">
         <v>1</v>
       </c>
-      <c r="F35" s="3">
-        <v>0</v>
-      </c>
       <c r="G35" s="3">
+        <v>0</v>
+      </c>
+      <c r="H35" s="3">
         <v>1</v>
       </c>
-      <c r="H35" s="3">
-        <v>0</v>
-      </c>
       <c r="I35" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B36" s="3">
         <v>1</v>
@@ -29294,7 +29326,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B37" s="3">
         <v>1</v>
@@ -29323,7 +29355,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A38" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B38" s="3">
         <v>1</v>
@@ -29352,59 +29384,30 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A39" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B39" s="3">
         <v>1</v>
       </c>
       <c r="C39" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D39" s="3">
         <v>1</v>
       </c>
       <c r="E39" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F39" s="3">
         <v>1</v>
       </c>
       <c r="G39" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H39" s="3">
         <v>1</v>
       </c>
       <c r="I39" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A40" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B40" s="3">
-        <v>1</v>
-      </c>
-      <c r="C40" s="3">
-        <v>1</v>
-      </c>
-      <c r="D40" s="3">
-        <v>1</v>
-      </c>
-      <c r="E40" s="3">
-        <v>1</v>
-      </c>
-      <c r="F40" s="3">
-        <v>1</v>
-      </c>
-      <c r="G40" s="3">
-        <v>1</v>
-      </c>
-      <c r="H40" s="3">
-        <v>1</v>
-      </c>
-      <c r="I40" s="3">
         <v>1</v>
       </c>
     </row>
@@ -29418,8 +29421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7CDD2E9-B0AB-4B78-AAF0-949DF9D7B865}">
   <dimension ref="A1:AN1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H49" sqref="H49"/>
+    <sheetView topLeftCell="L1" zoomScale="92" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="AG1" sqref="AG1:AL1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -32319,7 +32322,7 @@
         <v>0</v>
       </c>
       <c r="H25" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I25" s="3">
         <v>0</v>
@@ -34207,15 +34210,15 @@
     <row r="43" spans="1:39" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
-      <c r="C43" s="8" t="s">
+      <c r="C43" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D43" s="11" t="s">
+      <c r="D43" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="E43" s="12"/>
-      <c r="F43" s="12"/>
-      <c r="G43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="14"/>
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
       <c r="J43" s="3"/>
@@ -34252,7 +34255,7 @@
     <row r="44" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
-      <c r="C44" s="9"/>
+      <c r="C44" s="10"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
@@ -34291,16 +34294,16 @@
       <c r="AM44" s="3"/>
     </row>
     <row r="45" spans="1:39" x14ac:dyDescent="0.45">
-      <c r="C45" s="9"/>
+      <c r="C45" s="10"/>
     </row>
     <row r="46" spans="1:39" x14ac:dyDescent="0.45">
-      <c r="C46" s="9"/>
+      <c r="C46" s="10"/>
     </row>
     <row r="47" spans="1:39" x14ac:dyDescent="0.45">
-      <c r="C47" s="9"/>
+      <c r="C47" s="10"/>
     </row>
     <row r="48" spans="1:39" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C48" s="10"/>
+      <c r="C48" s="11"/>
     </row>
     <row r="50" spans="1:40" x14ac:dyDescent="0.45">
       <c r="B50" s="7"/>
@@ -73506,15 +73509,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2805CA7-F238-4F23-AF6C-90621E1D8A57}">
-  <dimension ref="A1:AG33"/>
+  <dimension ref="A1:AM40"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="X41" sqref="X41"/>
+    <sheetView tabSelected="1" zoomScale="156" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="10.796875" style="8" customWidth="1"/>
+    <col min="2" max="39" width="10.796875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:39" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="3"/>
       <c r="B1" s="3" t="s">
         <v>10</v>
@@ -73612,8 +73619,26 @@
       <c r="AG1" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="AH1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AI1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AL1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AM1" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -73713,8 +73738,26 @@
       <c r="AG2" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="AH2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -73814,8 +73857,26 @@
       <c r="AG3" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="AH3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -73915,8 +73976,26 @@
       <c r="AG4" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:33" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="AH4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:39" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -74016,8 +74095,26 @@
       <c r="AG5" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="AH5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM5" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
@@ -74117,8 +74214,26 @@
       <c r="AG6" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:33" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="AH6" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI6" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ6" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK6" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL6" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM6" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:39" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
@@ -74218,8 +74333,26 @@
       <c r="AG7" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:33" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="AH7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM7" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:39" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
@@ -74319,8 +74452,26 @@
       <c r="AG8" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:33" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="AH8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM8" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:39" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
@@ -74420,8 +74571,26 @@
       <c r="AG9" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:33" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="AH9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM9" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:39" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
@@ -74521,8 +74690,26 @@
       <c r="AG10" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="AH10" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI10" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ10" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK10" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL10" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM10" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
@@ -74622,8 +74809,26 @@
       <c r="AG11" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:33" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="AH11" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI11" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ11" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK11" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL11" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
         <v>20</v>
       </c>
@@ -74723,8 +74928,26 @@
       <c r="AG12" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:33" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="AH12" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI12" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ12" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK12" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL12" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM12" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:39" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
         <v>21</v>
       </c>
@@ -74824,8 +75047,26 @@
       <c r="AG13" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="AH13" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI13" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ13" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK13" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL13" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
         <v>47</v>
       </c>
@@ -74925,8 +75166,26 @@
       <c r="AG14" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="AH14" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI14" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ14" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK14" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL14" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM14" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>22</v>
       </c>
@@ -75026,8 +75285,26 @@
       <c r="AG15" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:33" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="AH15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM15" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:39" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
         <v>23</v>
       </c>
@@ -75127,8 +75404,26 @@
       <c r="AG16" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:33" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="AH16" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI16" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ16" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK16" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL16" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM16" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:39" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
         <v>24</v>
       </c>
@@ -75228,8 +75523,26 @@
       <c r="AG17" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:33" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="AH17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM17" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:39" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
         <v>25</v>
       </c>
@@ -75329,8 +75642,26 @@
       <c r="AG18" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="AH18" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI18" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ18" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK18" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL18" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM18" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
         <v>26</v>
       </c>
@@ -75430,8 +75761,26 @@
       <c r="AG19" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="AH19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM19" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
         <v>27</v>
       </c>
@@ -75531,8 +75880,26 @@
       <c r="AG20" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="AH20" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI20" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ20" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK20" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL20" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM20" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
         <v>28</v>
       </c>
@@ -75632,8 +75999,26 @@
       <c r="AG21" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="AH21" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI21" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ21" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK21" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL21" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM21" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
         <v>29</v>
       </c>
@@ -75733,8 +76118,26 @@
       <c r="AG22" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="AH22" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI22" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ22" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK22" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL22" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM22" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
         <v>30</v>
       </c>
@@ -75834,8 +76237,26 @@
       <c r="AG23" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="AH23" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI23" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ23" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK23" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL23" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM23" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
         <v>31</v>
       </c>
@@ -75935,8 +76356,26 @@
       <c r="AG24" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="AH24" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI24" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ24" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK24" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL24" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM24" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
         <v>32</v>
       </c>
@@ -76036,8 +76475,26 @@
       <c r="AG25" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="AH25" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI25" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ25" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK25" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL25" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM25" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A26" s="3" t="s">
         <v>33</v>
       </c>
@@ -76060,7 +76517,7 @@
         <v>0</v>
       </c>
       <c r="H26" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26" s="3">
         <v>0</v>
@@ -76137,8 +76594,26 @@
       <c r="AG26" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="AH26" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI26" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ26" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK26" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL26" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM26" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A27" s="3" t="s">
         <v>34</v>
       </c>
@@ -76238,8 +76713,26 @@
       <c r="AG27" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="AH27" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI27" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ27" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK27" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL27" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM27" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A28" s="3" t="s">
         <v>35</v>
       </c>
@@ -76339,8 +76832,26 @@
       <c r="AG28" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="AH28" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI28" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ28" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK28" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL28" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM28" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A29" s="3" t="s">
         <v>36</v>
       </c>
@@ -76440,8 +76951,26 @@
       <c r="AG29" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="AH29" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI29" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ29" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK29" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL29" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM29" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A30" s="3" t="s">
         <v>37</v>
       </c>
@@ -76541,8 +77070,26 @@
       <c r="AG30" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="AH30" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI30" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ30" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK30" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL30" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM30" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A31" s="3" t="s">
         <v>38</v>
       </c>
@@ -76642,8 +77189,26 @@
       <c r="AG31" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="AH31" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI31" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ31" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK31" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL31" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM31" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A32" s="3" t="s">
         <v>39</v>
       </c>
@@ -76743,8 +77308,26 @@
       <c r="AG32" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="AH32" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI32" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ32" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK32" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL32" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM32" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A33" s="3" t="s">
         <v>40</v>
       </c>
@@ -76844,6 +77427,741 @@
       <c r="AG33" s="3">
         <v>0</v>
       </c>
+      <c r="AH33" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI33" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ33" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK33" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL33" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM33" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:39" x14ac:dyDescent="0.45">
+      <c r="A34" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" s="3">
+        <v>0</v>
+      </c>
+      <c r="C34" s="3">
+        <v>0</v>
+      </c>
+      <c r="D34" s="3">
+        <v>0</v>
+      </c>
+      <c r="E34" s="3">
+        <v>0</v>
+      </c>
+      <c r="F34" s="3">
+        <v>0</v>
+      </c>
+      <c r="G34" s="3">
+        <v>0</v>
+      </c>
+      <c r="H34" s="3">
+        <v>0</v>
+      </c>
+      <c r="I34" s="3">
+        <v>0</v>
+      </c>
+      <c r="J34" s="3">
+        <v>0</v>
+      </c>
+      <c r="K34" s="3">
+        <v>0</v>
+      </c>
+      <c r="L34" s="3">
+        <v>0</v>
+      </c>
+      <c r="M34" s="3">
+        <v>0</v>
+      </c>
+      <c r="N34" s="3">
+        <v>0</v>
+      </c>
+      <c r="O34" s="3">
+        <v>0</v>
+      </c>
+      <c r="P34" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="3">
+        <v>0</v>
+      </c>
+      <c r="R34" s="3">
+        <v>0</v>
+      </c>
+      <c r="S34" s="3">
+        <v>0</v>
+      </c>
+      <c r="T34" s="3">
+        <v>0</v>
+      </c>
+      <c r="U34" s="3">
+        <v>0</v>
+      </c>
+      <c r="V34" s="3">
+        <v>0</v>
+      </c>
+      <c r="W34" s="3">
+        <v>0</v>
+      </c>
+      <c r="X34" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y34" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z34" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA34" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB34" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC34" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD34" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE34" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF34" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG34" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH34" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI34" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ34" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK34" s="3">
+        <v>0</v>
+      </c>
+      <c r="AL34" s="3">
+        <v>0</v>
+      </c>
+      <c r="AM34" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:39" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A35" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35" s="3">
+        <v>0</v>
+      </c>
+      <c r="C35" s="3">
+        <v>0</v>
+      </c>
+      <c r="D35" s="3">
+        <v>0</v>
+      </c>
+      <c r="E35" s="3">
+        <v>0</v>
+      </c>
+      <c r="F35" s="3">
+        <v>0</v>
+      </c>
+      <c r="G35" s="3">
+        <v>0</v>
+      </c>
+      <c r="H35" s="3">
+        <v>0</v>
+      </c>
+      <c r="I35" s="3">
+        <v>0</v>
+      </c>
+      <c r="J35" s="3">
+        <v>0</v>
+      </c>
+      <c r="K35" s="3">
+        <v>0</v>
+      </c>
+      <c r="L35" s="3">
+        <v>0</v>
+      </c>
+      <c r="M35" s="3">
+        <v>0</v>
+      </c>
+      <c r="N35" s="3">
+        <v>0</v>
+      </c>
+      <c r="O35" s="3">
+        <v>0</v>
+      </c>
+      <c r="P35" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="3">
+        <v>0</v>
+      </c>
+      <c r="R35" s="3">
+        <v>0</v>
+      </c>
+      <c r="S35" s="3">
+        <v>0</v>
+      </c>
+      <c r="T35" s="3">
+        <v>0</v>
+      </c>
+      <c r="U35" s="3">
+        <v>0</v>
+      </c>
+      <c r="V35" s="3">
+        <v>0</v>
+      </c>
+      <c r="W35" s="3">
+        <v>1</v>
+      </c>
+      <c r="X35" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y35" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z35" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA35" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB35" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC35" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD35" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE35" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF35" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG35" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH35" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI35" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ35" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK35" s="3">
+        <v>0</v>
+      </c>
+      <c r="AL35" s="3">
+        <v>0</v>
+      </c>
+      <c r="AM35" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:39" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A36" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36" s="3">
+        <v>0</v>
+      </c>
+      <c r="C36" s="3">
+        <v>0</v>
+      </c>
+      <c r="D36" s="3">
+        <v>0</v>
+      </c>
+      <c r="E36" s="3">
+        <v>0</v>
+      </c>
+      <c r="F36" s="3">
+        <v>0</v>
+      </c>
+      <c r="G36" s="3">
+        <v>0</v>
+      </c>
+      <c r="H36" s="3">
+        <v>0</v>
+      </c>
+      <c r="I36" s="3">
+        <v>0</v>
+      </c>
+      <c r="J36" s="3">
+        <v>0</v>
+      </c>
+      <c r="K36" s="3">
+        <v>0</v>
+      </c>
+      <c r="L36" s="3">
+        <v>0</v>
+      </c>
+      <c r="M36" s="3">
+        <v>0</v>
+      </c>
+      <c r="N36" s="3">
+        <v>0</v>
+      </c>
+      <c r="O36" s="3">
+        <v>0</v>
+      </c>
+      <c r="P36" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="3">
+        <v>0</v>
+      </c>
+      <c r="R36" s="3">
+        <v>0</v>
+      </c>
+      <c r="S36" s="3">
+        <v>0</v>
+      </c>
+      <c r="T36" s="3">
+        <v>0</v>
+      </c>
+      <c r="U36" s="3">
+        <v>0</v>
+      </c>
+      <c r="V36" s="3">
+        <v>0</v>
+      </c>
+      <c r="W36" s="3">
+        <v>0</v>
+      </c>
+      <c r="X36" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y36" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z36" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA36" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB36" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC36" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD36" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE36" s="3">
+        <v>1</v>
+      </c>
+      <c r="AF36" s="3">
+        <v>1</v>
+      </c>
+      <c r="AG36" s="3">
+        <v>1</v>
+      </c>
+      <c r="AH36" s="3">
+        <v>1</v>
+      </c>
+      <c r="AI36" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ36" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK36" s="3">
+        <v>0</v>
+      </c>
+      <c r="AL36" s="3">
+        <v>0</v>
+      </c>
+      <c r="AM36" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:39" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A37" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37" s="3">
+        <v>0</v>
+      </c>
+      <c r="C37" s="3">
+        <v>0</v>
+      </c>
+      <c r="D37" s="3">
+        <v>0</v>
+      </c>
+      <c r="E37" s="3">
+        <v>0</v>
+      </c>
+      <c r="F37" s="3">
+        <v>0</v>
+      </c>
+      <c r="G37" s="3">
+        <v>0</v>
+      </c>
+      <c r="H37" s="3">
+        <v>0</v>
+      </c>
+      <c r="I37" s="3">
+        <v>0</v>
+      </c>
+      <c r="J37" s="3">
+        <v>0</v>
+      </c>
+      <c r="K37" s="3">
+        <v>0</v>
+      </c>
+      <c r="L37" s="3">
+        <v>0</v>
+      </c>
+      <c r="M37" s="3">
+        <v>0</v>
+      </c>
+      <c r="N37" s="3">
+        <v>0</v>
+      </c>
+      <c r="O37" s="3">
+        <v>0</v>
+      </c>
+      <c r="P37" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="3">
+        <v>0</v>
+      </c>
+      <c r="R37" s="3">
+        <v>0</v>
+      </c>
+      <c r="S37" s="3">
+        <v>0</v>
+      </c>
+      <c r="T37" s="3">
+        <v>0</v>
+      </c>
+      <c r="U37" s="3">
+        <v>0</v>
+      </c>
+      <c r="V37" s="3">
+        <v>0</v>
+      </c>
+      <c r="W37" s="3">
+        <v>0</v>
+      </c>
+      <c r="X37" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y37" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z37" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA37" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB37" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC37" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD37" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE37" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF37" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG37" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH37" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI37" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ37" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK37" s="3">
+        <v>0</v>
+      </c>
+      <c r="AL37" s="3">
+        <v>0</v>
+      </c>
+      <c r="AM37" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:39" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A38" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" s="3">
+        <v>0</v>
+      </c>
+      <c r="C38" s="3">
+        <v>0</v>
+      </c>
+      <c r="D38" s="3">
+        <v>0</v>
+      </c>
+      <c r="E38" s="3">
+        <v>0</v>
+      </c>
+      <c r="F38" s="3">
+        <v>0</v>
+      </c>
+      <c r="G38" s="3">
+        <v>0</v>
+      </c>
+      <c r="H38" s="3">
+        <v>0</v>
+      </c>
+      <c r="I38" s="3">
+        <v>0</v>
+      </c>
+      <c r="J38" s="3">
+        <v>0</v>
+      </c>
+      <c r="K38" s="3">
+        <v>0</v>
+      </c>
+      <c r="L38" s="3">
+        <v>0</v>
+      </c>
+      <c r="M38" s="3">
+        <v>0</v>
+      </c>
+      <c r="N38" s="3">
+        <v>0</v>
+      </c>
+      <c r="O38" s="3">
+        <v>0</v>
+      </c>
+      <c r="P38" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q38" s="3">
+        <v>0</v>
+      </c>
+      <c r="R38" s="3">
+        <v>0</v>
+      </c>
+      <c r="S38" s="3">
+        <v>0</v>
+      </c>
+      <c r="T38" s="3">
+        <v>0</v>
+      </c>
+      <c r="U38" s="3">
+        <v>0</v>
+      </c>
+      <c r="V38" s="3">
+        <v>0</v>
+      </c>
+      <c r="W38" s="3">
+        <v>0</v>
+      </c>
+      <c r="X38" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y38" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z38" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA38" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB38" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC38" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD38" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE38" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF38" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG38" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH38" s="3">
+        <v>1</v>
+      </c>
+      <c r="AI38" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ38" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK38" s="3">
+        <v>0</v>
+      </c>
+      <c r="AL38" s="3">
+        <v>0</v>
+      </c>
+      <c r="AM38" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:39" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A39" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B39" s="3">
+        <v>0</v>
+      </c>
+      <c r="C39" s="3">
+        <v>0</v>
+      </c>
+      <c r="D39" s="3">
+        <v>0</v>
+      </c>
+      <c r="E39" s="3">
+        <v>0</v>
+      </c>
+      <c r="F39" s="3">
+        <v>0</v>
+      </c>
+      <c r="G39" s="3">
+        <v>0</v>
+      </c>
+      <c r="H39" s="3">
+        <v>0</v>
+      </c>
+      <c r="I39" s="3">
+        <v>0</v>
+      </c>
+      <c r="J39" s="3">
+        <v>0</v>
+      </c>
+      <c r="K39" s="3">
+        <v>0</v>
+      </c>
+      <c r="L39" s="3">
+        <v>0</v>
+      </c>
+      <c r="M39" s="3">
+        <v>0</v>
+      </c>
+      <c r="N39" s="3">
+        <v>0</v>
+      </c>
+      <c r="O39" s="3">
+        <v>0</v>
+      </c>
+      <c r="P39" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q39" s="3">
+        <v>0</v>
+      </c>
+      <c r="R39" s="3">
+        <v>0</v>
+      </c>
+      <c r="S39" s="3">
+        <v>0</v>
+      </c>
+      <c r="T39" s="3">
+        <v>0</v>
+      </c>
+      <c r="U39" s="3">
+        <v>0</v>
+      </c>
+      <c r="V39" s="3">
+        <v>0</v>
+      </c>
+      <c r="W39" s="3">
+        <v>0</v>
+      </c>
+      <c r="X39" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y39" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z39" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA39" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB39" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC39" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD39" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE39" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF39" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG39" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH39" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI39" s="3">
+        <v>1</v>
+      </c>
+      <c r="AJ39" s="3">
+        <v>1</v>
+      </c>
+      <c r="AK39" s="3">
+        <v>1</v>
+      </c>
+      <c r="AL39" s="3">
+        <v>1</v>
+      </c>
+      <c r="AM39" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:39" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A40" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>